<commit_message>
Giải thích Thiên Di
</commit_message>
<xml_diff>
--- a/LuanThienDi.xlsx
+++ b/LuanThienDi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A11D76F-A8AA-4437-AC06-1E5C1FE42521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367E8BE6-C2B7-4504-9E48-11FC75FF8BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8760" uniqueCount="4417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8774" uniqueCount="4446">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13278,6 +13278,93 @@
   </si>
   <si>
     <t>Hay mắc tai nạn, xa nhà rất bất lợi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ra ngoài được nhiều người vị nể, tài lộc dễ kiếm, lời nói được nhiều người tin phục. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hay mắc thị phì kiện tụng và tai nạn nguy hiểm, sau này chết ở xa nhà. </t>
+  </si>
+  <si>
+    <t>Được nhiều người kính trọng, tài lộc dễ kiếm.</t>
+  </si>
+  <si>
+    <t>Xa nhà không được lợi ích tuy vậy vẫn được nhiều người mến chuộng</t>
+  </si>
+  <si>
+    <t>Được nhiều người kính trọng, yêu mến, hay lui tới những chỗ quyền qúy.</t>
+  </si>
+  <si>
+    <t>Gặp qúy nhân</t>
+  </si>
+  <si>
+    <t>Nay đây mai đó, chết ở xa nhà.</t>
+  </si>
+  <si>
+    <t>Thiên Cơ, Thiên Lương đồng cung tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Càng xa nhà càng gặp nhiều may mắn, hay được lui tới chỗ quyền qúy, được nhiều người tôn kính vị nể.</t>
+  </si>
+  <si>
+    <t>Hay gặp qúy nhân, vì có oai nên được nhiều người kính nể, lời nói được nhiều người tin phục, hay lui tới những chỗ có uy quyền.</t>
+  </si>
+  <si>
+    <t>Được nhiều nể sợ và tin phục. Thường gần nơi quyền qúy nhưng không nên ra ngoài nhiều, vì may thường đi liền với rủi, hay mắc tai nạn, sau này chết xa nhà</t>
+  </si>
+  <si>
+    <t>Ra ngoài rất bất lợi. Lúc chết không được ở gần nhà.</t>
+  </si>
+  <si>
+    <t>Nhiều người nể sợ, tài lộc dễ kiếm, nhưng đôi khi mắc tai nạn nguy hiểm.</t>
+  </si>
+  <si>
+    <t>Hay mắc tai nạn nhất là về xe cộ và ác thú, hay gặp những kẻ rình ám hại. Nếu hay xoay sở tiền tài lại càng dễ gặp tai họa, sau này chết ở xa nhà.</t>
+  </si>
+  <si>
+    <t>May đi liền với rủi, người kính trọng cũng có mà ghen ghét muốn hại cũng nhiều. Tai ương đầy rẫy nhưng vẫn ưa thích nay đây mai đó. Sau chết ở xa nhà</t>
+  </si>
+  <si>
+    <t>Hay mắc tai nạn. Sau này chết ở xa nhà.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hung họa đầy rẫy, hay mắc thị phi, khó kiếm tiền, luôn gặp những sự phiền lòng. </t>
+  </si>
+  <si>
+    <t>Kình Dương, Đà La sáng sủa hội chiếu tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Kình Dương, Đà La tối tăm hội chiếu tại Thiên Di</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dễ kiếm tiền, tuy hay gặp qúy nhân nhưng vẫn bị nhiều người khinh bỉ. </t>
+  </si>
+  <si>
+    <t>Hỏa Linh</t>
+  </si>
+  <si>
+    <t>Hỏa Linh hội chiếu tại Thiên Di</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ra ngoài chẳng được yên chân. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hay bị lừa đảo, mưu hại, lúc chết không ở gần nhà. </t>
+  </si>
+  <si>
+    <t>Gặp nhiều qúy nhàn. Thường được gần những bậc quyến cao, chức trọng.</t>
+  </si>
+  <si>
+    <t>Gặp nhiều người giúp đỡ.</t>
+  </si>
+  <si>
+    <t>Lộc Tồn Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Lộc Tồn Hóa Lộc hội chiếu tại Thiên Di</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dễ kiếm tiền, luôn luôn gặp may mắn, buôn bán phát tài </t>
   </si>
 </sst>
 </file>
@@ -13331,297 +13418,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="64">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="35">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -14248,10 +14045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:D4378"/>
+  <dimension ref="A1:D4385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4362" workbookViewId="0">
-      <selection activeCell="J4369" sqref="J4369"/>
+    <sheetView tabSelected="1" topLeftCell="A4369" workbookViewId="0">
+      <selection activeCell="F4373" sqref="F4373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21419,12 +21216,12 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="896" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="896" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A896" s="1" t="s">
         <v>1025</v>
       </c>
       <c r="B896" s="1" t="s">
-        <v>1025</v>
+        <v>4402</v>
       </c>
     </row>
     <row r="897" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -21451,12 +21248,12 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="900" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="900" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A900" s="1" t="s">
         <v>1029</v>
       </c>
       <c r="B900" s="1" t="s">
-        <v>1029</v>
+        <v>4402</v>
       </c>
     </row>
     <row r="901" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -21547,12 +21344,12 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="912" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="912" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A912" s="1" t="s">
         <v>1041</v>
       </c>
       <c r="B912" s="1" t="s">
-        <v>1041</v>
+        <v>4402</v>
       </c>
     </row>
     <row r="913" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -21579,12 +21376,12 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="916" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="916" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A916" s="1" t="s">
         <v>1045</v>
       </c>
       <c r="B916" s="1" t="s">
-        <v>1045</v>
+        <v>4402</v>
       </c>
     </row>
     <row r="917" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -24747,12 +24544,12 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="1312" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1312" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1312" s="1" t="s">
         <v>1422</v>
       </c>
       <c r="B1312" s="1" t="s">
-        <v>1422</v>
+        <v>4402</v>
       </c>
     </row>
     <row r="1313" spans="1:2" x14ac:dyDescent="0.25">
@@ -26715,12 +26512,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="1558" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1558" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1558" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B1558" s="1" t="s">
-        <v>39</v>
+        <v>4420</v>
       </c>
     </row>
     <row r="1559" spans="1:2" x14ac:dyDescent="0.25">
@@ -34591,12 +34388,12 @@
         <v>2417</v>
       </c>
     </row>
-    <row r="2541" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2541" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2541" s="1" t="s">
         <v>2418</v>
       </c>
       <c r="B2541" s="1" t="s">
-        <v>2418</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="2542" spans="1:2" x14ac:dyDescent="0.25">
@@ -34623,28 +34420,28 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="2545" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2545" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2545" s="1" t="s">
         <v>2422</v>
       </c>
       <c r="B2545" s="1" t="s">
-        <v>2422</v>
-      </c>
-    </row>
-    <row r="2546" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4418</v>
+      </c>
+    </row>
+    <row r="2546" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2546" s="1" t="s">
         <v>2423</v>
       </c>
       <c r="B2546" s="1" t="s">
-        <v>2423</v>
-      </c>
-    </row>
-    <row r="2547" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4418</v>
+      </c>
+    </row>
+    <row r="2547" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2547" s="1" t="s">
         <v>2424</v>
       </c>
       <c r="B2547" s="1" t="s">
-        <v>2424</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="2548" spans="1:2" x14ac:dyDescent="0.25">
@@ -34671,20 +34468,20 @@
         <v>2427</v>
       </c>
     </row>
-    <row r="2551" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2551" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2551" s="1" t="s">
         <v>2428</v>
       </c>
       <c r="B2551" s="1" t="s">
-        <v>2428</v>
-      </c>
-    </row>
-    <row r="2552" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4418</v>
+      </c>
+    </row>
+    <row r="2552" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2552" s="1" t="s">
         <v>2429</v>
       </c>
       <c r="B2552" s="1" t="s">
-        <v>2429</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="2553" spans="1:2" x14ac:dyDescent="0.25">
@@ -34700,7 +34497,7 @@
         <v>2431</v>
       </c>
       <c r="B2554" s="1" t="s">
-        <v>2431</v>
+        <v>4419</v>
       </c>
     </row>
     <row r="2555" spans="1:2" x14ac:dyDescent="0.25">
@@ -34711,12 +34508,12 @@
         <v>2432</v>
       </c>
     </row>
-    <row r="2556" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2556" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2556" s="1" t="s">
         <v>2433</v>
       </c>
       <c r="B2556" s="1" t="s">
-        <v>2433</v>
+        <v>4420</v>
       </c>
     </row>
     <row r="2557" spans="1:2" x14ac:dyDescent="0.25">
@@ -34732,7 +34529,7 @@
         <v>2435</v>
       </c>
       <c r="B2558" s="1" t="s">
-        <v>2435</v>
+        <v>4419</v>
       </c>
     </row>
     <row r="2559" spans="1:2" x14ac:dyDescent="0.25">
@@ -34748,7 +34545,7 @@
         <v>2437</v>
       </c>
       <c r="B2560" s="1" t="s">
-        <v>2437</v>
+        <v>4419</v>
       </c>
     </row>
     <row r="2561" spans="1:2" x14ac:dyDescent="0.25">
@@ -34772,15 +34569,15 @@
         <v>2440</v>
       </c>
       <c r="B2563" s="1" t="s">
-        <v>2440</v>
-      </c>
-    </row>
-    <row r="2564" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4419</v>
+      </c>
+    </row>
+    <row r="2564" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2564" s="1" t="s">
         <v>2441</v>
       </c>
       <c r="B2564" s="1" t="s">
-        <v>2441</v>
+        <v>4421</v>
       </c>
     </row>
     <row r="2565" spans="1:2" x14ac:dyDescent="0.25">
@@ -34788,7 +34585,7 @@
         <v>2442</v>
       </c>
       <c r="B2565" s="1" t="s">
-        <v>2442</v>
+        <v>4422</v>
       </c>
     </row>
     <row r="2566" spans="1:2" x14ac:dyDescent="0.25">
@@ -34820,15 +34617,15 @@
         <v>2446</v>
       </c>
       <c r="B2569" s="1" t="s">
-        <v>2446</v>
-      </c>
-    </row>
-    <row r="2570" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4423</v>
+      </c>
+    </row>
+    <row r="2570" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2570" s="1" t="s">
         <v>2447</v>
       </c>
       <c r="B2570" s="1" t="s">
-        <v>2447</v>
+        <v>4421</v>
       </c>
     </row>
     <row r="2571" spans="1:2" x14ac:dyDescent="0.25">
@@ -34836,7 +34633,7 @@
         <v>2448</v>
       </c>
       <c r="B2571" s="1" t="s">
-        <v>2448</v>
+        <v>4422</v>
       </c>
     </row>
     <row r="2572" spans="1:2" x14ac:dyDescent="0.25">
@@ -34868,15 +34665,15 @@
         <v>2452</v>
       </c>
       <c r="B2575" s="1" t="s">
-        <v>2452</v>
-      </c>
-    </row>
-    <row r="2576" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4423</v>
+      </c>
+    </row>
+    <row r="2576" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2576" s="1" t="s">
         <v>2453</v>
       </c>
       <c r="B2576" s="1" t="s">
-        <v>2453</v>
+        <v>4427</v>
       </c>
     </row>
     <row r="2577" spans="1:2" x14ac:dyDescent="0.25">
@@ -34887,12 +34684,12 @@
         <v>2454</v>
       </c>
     </row>
-    <row r="2578" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2578" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2578" s="1" t="s">
         <v>2455</v>
       </c>
       <c r="B2578" s="1" t="s">
-        <v>2455</v>
+        <v>4426</v>
       </c>
     </row>
     <row r="2579" spans="1:2" x14ac:dyDescent="0.25">
@@ -34908,7 +34705,7 @@
         <v>2457</v>
       </c>
       <c r="B2580" s="1" t="s">
-        <v>2457</v>
+        <v>4428</v>
       </c>
     </row>
     <row r="2581" spans="1:2" x14ac:dyDescent="0.25">
@@ -34919,12 +34716,12 @@
         <v>2458</v>
       </c>
     </row>
-    <row r="2582" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2582" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2582" s="1" t="s">
         <v>2459</v>
       </c>
       <c r="B2582" s="1" t="s">
-        <v>2459</v>
+        <v>4427</v>
       </c>
     </row>
     <row r="2583" spans="1:2" x14ac:dyDescent="0.25">
@@ -34935,12 +34732,12 @@
         <v>2460</v>
       </c>
     </row>
-    <row r="2584" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2584" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2584" s="1" t="s">
         <v>2461</v>
       </c>
       <c r="B2584" s="1" t="s">
-        <v>2461</v>
+        <v>4426</v>
       </c>
     </row>
     <row r="2585" spans="1:2" x14ac:dyDescent="0.25">
@@ -34956,7 +34753,7 @@
         <v>2463</v>
       </c>
       <c r="B2586" s="1" t="s">
-        <v>2463</v>
+        <v>4428</v>
       </c>
     </row>
     <row r="2587" spans="1:2" x14ac:dyDescent="0.25">
@@ -34967,12 +34764,12 @@
         <v>2464</v>
       </c>
     </row>
-    <row r="2588" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2588" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2588" s="1" t="s">
         <v>2465</v>
       </c>
       <c r="B2588" s="1" t="s">
-        <v>2465</v>
+        <v>4429</v>
       </c>
     </row>
     <row r="2589" spans="1:2" x14ac:dyDescent="0.25">
@@ -34983,12 +34780,12 @@
         <v>2466</v>
       </c>
     </row>
-    <row r="2590" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2590" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2590" s="1" t="s">
         <v>2467</v>
       </c>
       <c r="B2590" s="1" t="s">
-        <v>2467</v>
+        <v>4430</v>
       </c>
     </row>
     <row r="2591" spans="1:2" x14ac:dyDescent="0.25">
@@ -34999,12 +34796,12 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="2592" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2592" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2592" s="1" t="s">
         <v>2469</v>
       </c>
       <c r="B2592" s="1" t="s">
-        <v>2469</v>
+        <v>4431</v>
       </c>
     </row>
     <row r="2593" spans="1:2" x14ac:dyDescent="0.25">
@@ -35015,12 +34812,12 @@
         <v>2470</v>
       </c>
     </row>
-    <row r="2594" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2594" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2594" s="1" t="s">
         <v>2471</v>
       </c>
       <c r="B2594" s="1" t="s">
-        <v>2471</v>
+        <v>4429</v>
       </c>
     </row>
     <row r="2595" spans="1:2" x14ac:dyDescent="0.25">
@@ -35031,12 +34828,12 @@
         <v>2472</v>
       </c>
     </row>
-    <row r="2596" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2596" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2596" s="1" t="s">
         <v>2473</v>
       </c>
       <c r="B2596" s="1" t="s">
-        <v>2473</v>
+        <v>4430</v>
       </c>
     </row>
     <row r="2597" spans="1:2" x14ac:dyDescent="0.25">
@@ -47716,7 +47513,7 @@
         <v>4179</v>
       </c>
       <c r="B4181" s="1" t="s">
-        <v>4179</v>
+        <v>4432</v>
       </c>
     </row>
     <row r="4182" spans="1:2" x14ac:dyDescent="0.25">
@@ -47740,7 +47537,7 @@
         <v>4182</v>
       </c>
       <c r="B4184" s="1" t="s">
-        <v>4182</v>
+        <v>4440</v>
       </c>
     </row>
     <row r="4185" spans="1:2" x14ac:dyDescent="0.25">
@@ -47756,7 +47553,7 @@
         <v>4184</v>
       </c>
       <c r="B4186" s="1" t="s">
-        <v>4184</v>
+        <v>4442</v>
       </c>
     </row>
     <row r="4187" spans="1:2" x14ac:dyDescent="0.25">
@@ -48135,12 +47932,12 @@
         <v>4231</v>
       </c>
     </row>
-    <row r="4234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4234" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4234" s="1" t="s">
         <v>4232</v>
       </c>
       <c r="B4234" s="1" t="s">
-        <v>4232</v>
+        <v>4433</v>
       </c>
     </row>
     <row r="4235" spans="1:2" x14ac:dyDescent="0.25">
@@ -48207,12 +48004,12 @@
         <v>4240</v>
       </c>
     </row>
-    <row r="4243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4243" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4243" s="1" t="s">
         <v>4241</v>
       </c>
       <c r="B4243" s="1" t="s">
-        <v>4241</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="4244" spans="1:2" x14ac:dyDescent="0.25">
@@ -49295,93 +49092,152 @@
         <v>4387</v>
       </c>
     </row>
+    <row r="4379" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4379" s="1" t="s">
+        <v>4424</v>
+      </c>
+      <c r="B4379" s="1" t="s">
+        <v>4425</v>
+      </c>
+    </row>
+    <row r="4380" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4380" s="1" t="s">
+        <v>4434</v>
+      </c>
+      <c r="B4380" s="1" t="s">
+        <v>4436</v>
+      </c>
+    </row>
+    <row r="4381" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4381" s="1" t="s">
+        <v>4435</v>
+      </c>
+      <c r="B4381" s="1" t="s">
+        <v>4433</v>
+      </c>
+    </row>
+    <row r="4382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4382" s="1" t="s">
+        <v>4437</v>
+      </c>
+      <c r="B4382" s="1" t="s">
+        <v>4437</v>
+      </c>
+    </row>
+    <row r="4383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4383" s="1" t="s">
+        <v>4438</v>
+      </c>
+      <c r="B4383" s="1" t="s">
+        <v>4439</v>
+      </c>
+    </row>
+    <row r="4384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4384" s="1" t="s">
+        <v>4443</v>
+      </c>
+      <c r="B4384" s="1" t="s">
+        <v>4443</v>
+      </c>
+    </row>
+    <row r="4385" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4385" s="1" t="s">
+        <v>4444</v>
+      </c>
+      <c r="B4385" s="1" t="s">
+        <v>4445</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="33" priority="104"/>
-    <cfRule type="duplicateValues" dxfId="32" priority="105"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="105"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="106"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="31" priority="74"/>
-    <cfRule type="duplicateValues" dxfId="30" priority="75"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="75"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="76"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="29" priority="78"/>
-    <cfRule type="duplicateValues" dxfId="28" priority="79"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="79"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="80"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145:A208">
-    <cfRule type="duplicateValues" dxfId="27" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6687:A1048576 A1769:A1773 A209:A1600 A1:A23 A25:A84 A143 A3406:A3783 A3846:A4143 A1603:A1631">
-    <cfRule type="duplicateValues" dxfId="26" priority="113"/>
-    <cfRule type="duplicateValues" dxfId="25" priority="115"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="114"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="116"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1774:A3303">
-    <cfRule type="duplicateValues" dxfId="24" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3784:A3845">
-    <cfRule type="duplicateValues" dxfId="23" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="22" priority="20"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B142">
-    <cfRule type="duplicateValues" dxfId="20" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="18" priority="18"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145:B208">
+    <cfRule type="duplicateValues" dxfId="17" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6687:B1048576 B1769:B1773 B1:B23 B25:B84 B143 B3406:B3783 B3846:B4143 B1603:B1631 B209:B1600">
+    <cfRule type="duplicateValues" dxfId="2" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="24"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1774:B3303">
     <cfRule type="duplicateValues" dxfId="16" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6687:B1048576 B1769:B1773 B209:B1600 B1:B23 B25:B84 B143 B3406:B3783 B3846:B4143 B1603:B1631">
-    <cfRule type="duplicateValues" dxfId="15" priority="22"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="23"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1774:B3303">
-    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B3784:B3845">
-    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1601">
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1601">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1601">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1601">
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1602">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1602">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1602">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1602">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1647">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B136">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B141">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1558">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
giải xong thiên di
</commit_message>
<xml_diff>
--- a/LuanThienDi.xlsx
+++ b/LuanThienDi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B9F90F-D2D1-4B12-A9F8-055D2C9D18E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664FDA39-F479-44A1-9BCE-B946984B0B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3375" yWindow="3375" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$B$4383</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$B$4380</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8770" uniqueCount="4479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8764" uniqueCount="4497">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -6669,9 +6669,6 @@
     <t>Thiên Sát tọa thủ tại Nô Bộc</t>
   </si>
   <si>
-    <t>Thiên Sát tọa thủ tại Thiên Di</t>
-  </si>
-  <si>
     <t>Thiên Sát tọa thủ tại Tật Ách</t>
   </si>
   <si>
@@ -6771,9 +6768,6 @@
     <t>Thiên Quang tọa thủ tại Nô Bộc</t>
   </si>
   <si>
-    <t>Thiên Quang tọa thủ tại Thiên Di</t>
-  </si>
-  <si>
     <t>Thiên Quang tọa thủ tại Tật Ách</t>
   </si>
   <si>
@@ -6937,9 +6931,6 @@
   </si>
   <si>
     <t>Quý Nhân tọa thủ tại Nô Bộc</t>
-  </si>
-  <si>
-    <t>Quý Nhân tọa thủ tại Thiên Di</t>
   </si>
   <si>
     <t>Quý Nhân tọa thủ tại Tật Ách</t>
@@ -13469,6 +13460,69 @@
   </si>
   <si>
     <t>Người ra ngoài khôn ngoan, nhiều được người mến chuộng nhưng khôn quá thì nhiều người ghét, và hãm hại. Người ra ngoài hay đi xa, cưới vợ xa quê.</t>
+  </si>
+  <si>
+    <t>Là người ra ngoài làm ăn vất vả, phải bon chen, đôi khi có sự gây gỗ, bực mình. Đi xa dễ trúng mánh làm ăn, phát dã như lôi nhưng thường không bền, đôi khi còn mất nhiều hơn được. Người có công danh vất vả, làm ăn lúc được lúc không, làm nghề cực nhọc. Người có số ly hương, đi xa, mồ côi, nếu không thì gia đạo cũng ly tán, xa cách. Người ra ngoài hay gặp tai họa, tai nạn bất ngờ, khó mà kiểm soát được, từ bên ngoài đem lại nên cần đặc biệt cẩn thận và tập cách bình tĩnh trước mọi sự việc xảy ra. Chủ về nghiệp duyên, ít được gặp duyên lành, sau này cưới vợ cưới chồng dễ bị yếu tố bên ngoài tác động mà bỏ nhau, không thì cũng dễ yểu thọ.</t>
+  </si>
+  <si>
+    <t>Là người ra ngoài vất vả, dù có gặp thuận lợi cũng không lâu bền, hay gặp tai nạn, trắc trở. Người hay bị các yếu tố ngoại cảnh bên ngoài gây tác động, ảnh hưởng tới tâm lý, suy tư dẫn tới căng thẳng đầu óc, các bệnh về thần kinh, trầm cảm… Người ra ngoài dễ thu hút vong tà đi theo về nhà, người hay lui tới các nơi tâm linh như đền chùa, miếu mạo…</t>
+  </si>
+  <si>
+    <t>Là người ra ngoài không có nơi chốn cố định, đa nghệ. Người ra ngoài hay thích tới những nơi ăn chơi, nhục dục, nhiều mối quan hệ không lành mạnh, tình một đêm. Người ra ngoài hay dễ có ma tà, vong theo về. Người thích đi xem bói toán, đi đền đi chùa…</t>
+  </si>
+  <si>
+    <t>Người ra ngoài khiêm tốn, hay gặp quý nhân giúp đỡ. Người ra ngoài nổi tiếng, nhiều người khác giới hâm mộ. Người hay phải đi xa lập nghiệp</t>
+  </si>
+  <si>
+    <t>Ra ngoài thường cư xử nhẹ nhàng, khiêm tốn, tốt bụng, ôn hòa, gần gũi hay giúp đỡ mọi người chia sẻ những điều tốt đẹp đến cho tất cả mọi người xung quanh nên được mọi người giúp đỡ, yêu mến và trân trọng. Người hay phải đi xa lập nghiệp</t>
+  </si>
+  <si>
+    <t>Là người ra ngoài có oai phong, được người mến chuộng, có quý nhân giúp đỡ. Người ra ngoài hanh thông, gặp nhiều thuận lợi, không phải cạnh tranh gay gắt, cho dù trong môi trường cạnh tranh gay gắt cũng được hanh thông nhàn nhã. Người ra ngoài, đi xa đạt được nhiều thành tựu, quý hiển, hay lui tới những nơi sang trọng, nhàn nhã. Người ra ngoài quan hệ rộng, đông người mến mộ, sẵn sàng giúp đỡ, hay đi nhiều nơi. Người ra ngoài không bao giờ phải làm việc nặng, thường nhẹ nhàng, thanh tao.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Người ra ngoài hay được mời, được rủ đi ăn đi uống, nhậu nhẹt nhiều. Ra ngoài, đi xa hay được may mắn, được quà tặng, khó khăn có người giúp đỡ.</t>
+  </si>
+  <si>
+    <t>Người ra ngoài có tài ăn nói lưu loát, thường được nhiều người khác giới để ý, đôi khi có thể ra ngoài được yêu quý bởi vì chính tài ăn nói của mình. Người ra ngoài phải cẩn thận vùng sông nước, nạn thủy tai. Đôi khi là hay phải đi tới những vùng sông nước nhiều khi ra ngoài. Người ra ngoài gặp nhiều kẻ hai mặt, bên ngoài thì ngọt nhẹ, bên trong thì nhiều mưu mô, toan tính, dễ lừa gạt nếu bản thân không cẩn thận.</t>
+  </si>
+  <si>
+    <t>Là người ra ngoài, đi xa hay gặp may mắn, được quý nhân giúp đỡ, thoát nạn.</t>
+  </si>
+  <si>
+    <t>Khi ra ngoài hay gặp chuyện phải tốn tiền, tổn hao nhiều. Người thường phải tha hương lập nghiệp, thay đổi chỗ ở nhiều lần, khó bền lâu được ở một nơi. Khi ra ngoài tốn tiền, thường phải tha hương lập nghiệp, thay đổi chỗ ở nhiều lần.</t>
+  </si>
+  <si>
+    <t>Khi ra ngoài hay gặp chuyện phải tốn tiền, tổn hao. Người thường phải tha hương lập nghiệp, thay đổi chỗ ở nhiều lần, khó lâu bền được ở một nơi.</t>
+  </si>
+  <si>
+    <t>Người ra ngoài dễ dính vào thị phi, kiện tụng. Gặp nhiều người khó tính khắt khe.</t>
+  </si>
+  <si>
+    <t>Bạn khi ra ngoài hay lo toan, làm công việc liên quan tới giấy tờ, văn bản, người ra ngoài hay diễn thuyết, thuyết trình.</t>
+  </si>
+  <si>
+    <t>Người tính mạnh mẽ, cương trực, thích uy quyền nên ra ngoài thường bị đố kỵ, cạnh tranh, ghen ghét, bị ám hại nếu đi với sao xấu. Người thẳng thắn, bộc tính nên thường ưa mềm mỏng, ra ngoài dễ bị người khác lừa.</t>
+  </si>
+  <si>
+    <t>Người hay phải đi lại nhiều, dễ xuất ngoại</t>
+  </si>
+  <si>
+    <t>Người ra ngoài khôn ngoan, cẩn thận, khiêm nhường, gặp nhiều may mắn. Người ra ngoài hay được mời đi ăn, rủ đi chơi xa.</t>
+  </si>
+  <si>
+    <t>Người ra ngoài thật thà, chân chất, hay giúp đỡ người.</t>
+  </si>
+  <si>
+    <t>E chừng có nhiều vấn đề không tốt, Mệnh sẽ có Phục binh là không tốt, cẩn thận số đi tù</t>
+  </si>
+  <si>
+    <t>Người ra ngoài luôn vui vẻ, hiền lành, được nhiều người tin tường và gặp nhiều may mắn. Người ra ngoài có nhiều người hâm mộ, quý mến và giúp đỡ.</t>
+  </si>
+  <si>
+    <t>Người ra ngoài, đi xa hay gặp may mắn, được quý nhân giúp đỡ, thoát nạn.</t>
+  </si>
+  <si>
+    <t>Người ra ngoài, đi xa thường hay gặp may mắn, thuận lợi trong công danh, thi cử, được trao tặng nhiều bằng cấp, khen thưởng. Người thuận lợi trong việc đi xa, có thể đi học xa, đi du học. Người ra ngoài gặp được quý nhân giúp đỡ, ra ngoài lợi ích hơn ở nhà.</t>
   </si>
 </sst>
 </file>
@@ -13504,12 +13558,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -14144,10 +14195,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D4383"/>
+  <dimension ref="A1:D4380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2027" workbookViewId="0">
-      <selection activeCell="D2037" sqref="D2037"/>
+    <sheetView tabSelected="1" topLeftCell="A1661" workbookViewId="0">
+      <selection activeCell="C1664" sqref="C1664"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14168,7 +14219,7 @@
         <v>141</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4444</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -14176,7 +14227,7 @@
         <v>142</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4445</v>
+        <v>4442</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -14184,7 +14235,7 @@
         <v>143</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4447</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -14192,7 +14243,7 @@
         <v>144</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4446</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -14200,7 +14251,7 @@
         <v>145</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4448</v>
+        <v>4445</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -14208,7 +14259,7 @@
         <v>146</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4449</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -15240,7 +15291,7 @@
         <v>273</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>4400</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -15280,7 +15331,7 @@
         <v>278</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>4400</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -15320,7 +15371,7 @@
         <v>283</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>4400</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -15360,7 +15411,7 @@
         <v>288</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>4400</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -15400,7 +15451,7 @@
         <v>293</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>4400</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -15536,7 +15587,7 @@
         <v>310</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>4401</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -15568,7 +15619,7 @@
         <v>314</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>4401</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -15600,7 +15651,7 @@
         <v>318</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>4401</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -15632,7 +15683,7 @@
         <v>322</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>4401</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -15765,10 +15816,10 @@
     </row>
     <row r="202" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>4403</v>
+        <v>4400</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>4404</v>
+        <v>4401</v>
       </c>
     </row>
     <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -21320,7 +21371,7 @@
         <v>1025</v>
       </c>
       <c r="B896" s="1" t="s">
-        <v>4400</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="897" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -21352,7 +21403,7 @@
         <v>1029</v>
       </c>
       <c r="B900" s="1" t="s">
-        <v>4400</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="901" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -21448,7 +21499,7 @@
         <v>1041</v>
       </c>
       <c r="B912" s="1" t="s">
-        <v>4400</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="913" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -21480,7 +21531,7 @@
         <v>1045</v>
       </c>
       <c r="B916" s="1" t="s">
-        <v>4400</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="917" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -24648,7 +24699,7 @@
         <v>1422</v>
       </c>
       <c r="B1312" s="1" t="s">
-        <v>4400</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="1313" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -26616,7 +26667,7 @@
         <v>39</v>
       </c>
       <c r="B1558" s="1" t="s">
-        <v>4418</v>
+        <v>4415</v>
       </c>
     </row>
     <row r="1559" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -26956,31 +27007,31 @@
       </c>
     </row>
     <row r="1601" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1601" s="2" t="s">
+      <c r="A1601" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B1601" s="1" t="s">
-        <v>4357</v>
+        <v>4354</v>
       </c>
       <c r="C1601" t="s">
-        <v>4358</v>
+        <v>4355</v>
       </c>
       <c r="D1601" t="s">
-        <v>4359</v>
+        <v>4356</v>
       </c>
     </row>
     <row r="1602" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1602" s="2" t="s">
+      <c r="A1602" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B1602" s="1" t="s">
-        <v>4357</v>
+        <v>4354</v>
       </c>
       <c r="C1602" t="s">
-        <v>4358</v>
+        <v>4355</v>
       </c>
       <c r="D1602" t="s">
-        <v>4359</v>
+        <v>4356</v>
       </c>
     </row>
     <row r="1603" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -26988,7 +27039,7 @@
         <v>84</v>
       </c>
       <c r="B1603" s="1" t="s">
-        <v>4450</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="1604" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -26996,7 +27047,7 @@
         <v>85</v>
       </c>
       <c r="B1604" s="1" t="s">
-        <v>4451</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="1605" spans="1:4" x14ac:dyDescent="0.25">
@@ -27340,7 +27391,7 @@
         <v>128</v>
       </c>
       <c r="B1647" s="1" t="s">
-        <v>4387</v>
+        <v>4384</v>
       </c>
     </row>
     <row r="1648" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -27460,7 +27511,7 @@
         <v>1660</v>
       </c>
       <c r="B1662" s="1" t="s">
-        <v>4452</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="1663" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -27468,7 +27519,7 @@
         <v>1661</v>
       </c>
       <c r="B1663" s="1" t="s">
-        <v>4452</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="1664" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -27476,7 +27527,7 @@
         <v>1662</v>
       </c>
       <c r="B1664" s="1" t="s">
-        <v>4453</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="1665" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -27484,7 +27535,7 @@
         <v>1663</v>
       </c>
       <c r="B1665" s="1" t="s">
-        <v>4453</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="1666" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -27572,7 +27623,7 @@
         <v>1674</v>
       </c>
       <c r="B1676" s="1" t="s">
-        <v>4454</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="1677" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -27660,7 +27711,7 @@
         <v>1685</v>
       </c>
       <c r="B1687" s="1" t="s">
-        <v>4454</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="1688" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -27756,7 +27807,7 @@
         <v>1697</v>
       </c>
       <c r="B1699" s="1" t="s">
-        <v>4455</v>
+        <v>4452</v>
       </c>
     </row>
     <row r="1700" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -27836,7 +27887,7 @@
         <v>1707</v>
       </c>
       <c r="B1709" s="1" t="s">
-        <v>4456</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="1710" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -27924,7 +27975,7 @@
         <v>1718</v>
       </c>
       <c r="B1720" s="1" t="s">
-        <v>4456</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="1721" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -28020,7 +28071,7 @@
         <v>1730</v>
       </c>
       <c r="B1732" s="1" t="s">
-        <v>4457</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="1733" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -28100,7 +28151,7 @@
         <v>1740</v>
       </c>
       <c r="B1742" s="1" t="s">
-        <v>4457</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="1743" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -28188,7 +28239,7 @@
         <v>1751</v>
       </c>
       <c r="B1753" s="1" t="s">
-        <v>4458</v>
+        <v>4455</v>
       </c>
     </row>
     <row r="1754" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -28276,7 +28327,7 @@
         <v>1762</v>
       </c>
       <c r="B1764" s="1" t="s">
-        <v>4459</v>
+        <v>4456</v>
       </c>
     </row>
     <row r="1765" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -28372,7 +28423,7 @@
         <v>1774</v>
       </c>
       <c r="B1776" s="1" t="s">
-        <v>4460</v>
+        <v>4457</v>
       </c>
     </row>
     <row r="1777" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -28540,7 +28591,7 @@
         <v>1795</v>
       </c>
       <c r="B1797" s="1" t="s">
-        <v>4461</v>
+        <v>4458</v>
       </c>
     </row>
     <row r="1798" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -28636,7 +28687,7 @@
         <v>1807</v>
       </c>
       <c r="B1809" s="1" t="s">
-        <v>4462</v>
+        <v>4459</v>
       </c>
     </row>
     <row r="1810" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -28716,7 +28767,7 @@
         <v>1817</v>
       </c>
       <c r="B1819" s="1" t="s">
-        <v>4463</v>
+        <v>4460</v>
       </c>
     </row>
     <row r="1820" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -28804,7 +28855,7 @@
         <v>1828</v>
       </c>
       <c r="B1830" s="1" t="s">
-        <v>4464</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="1831" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -28892,7 +28943,7 @@
         <v>1839</v>
       </c>
       <c r="B1841" s="1" t="s">
-        <v>4465</v>
+        <v>4462</v>
       </c>
     </row>
     <row r="1842" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -28988,7 +29039,7 @@
         <v>1851</v>
       </c>
       <c r="B1853" s="1" t="s">
-        <v>4466</v>
+        <v>4463</v>
       </c>
     </row>
     <row r="1854" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -29156,7 +29207,7 @@
         <v>1872</v>
       </c>
       <c r="B1874" s="1" t="s">
-        <v>4467</v>
+        <v>4464</v>
       </c>
     </row>
     <row r="1875" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -29252,7 +29303,7 @@
         <v>1884</v>
       </c>
       <c r="B1886" s="1" t="s">
-        <v>4467</v>
+        <v>4464</v>
       </c>
     </row>
     <row r="1887" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -29340,7 +29391,7 @@
         <v>1895</v>
       </c>
       <c r="B1897" s="1" t="s">
-        <v>4469</v>
+        <v>4466</v>
       </c>
     </row>
     <row r="1898" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -29428,7 +29479,7 @@
         <v>1906</v>
       </c>
       <c r="B1908" s="1" t="s">
-        <v>4468</v>
+        <v>4465</v>
       </c>
     </row>
     <row r="1909" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -29676,7 +29727,7 @@
         <v>1937</v>
       </c>
       <c r="B1939" s="1" t="s">
-        <v>4470</v>
+        <v>4467</v>
       </c>
     </row>
     <row r="1940" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -29756,7 +29807,7 @@
         <v>1947</v>
       </c>
       <c r="B1949" s="1" t="s">
-        <v>4470</v>
+        <v>4467</v>
       </c>
     </row>
     <row r="1950" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -29844,7 +29895,7 @@
         <v>1958</v>
       </c>
       <c r="B1960" s="1" t="s">
-        <v>4471</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="1961" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -29932,7 +29983,7 @@
         <v>1969</v>
       </c>
       <c r="B1971" s="1" t="s">
-        <v>4472</v>
+        <v>4469</v>
       </c>
     </row>
     <row r="1972" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -30020,7 +30071,7 @@
         <v>1980</v>
       </c>
       <c r="B1982" s="1" t="s">
-        <v>4473</v>
+        <v>4470</v>
       </c>
     </row>
     <row r="1983" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -30116,7 +30167,7 @@
         <v>1992</v>
       </c>
       <c r="B1994" s="1" t="s">
-        <v>4474</v>
+        <v>4471</v>
       </c>
     </row>
     <row r="1995" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -30204,7 +30255,7 @@
         <v>2003</v>
       </c>
       <c r="B2005" s="1" t="s">
-        <v>4475</v>
+        <v>4472</v>
       </c>
     </row>
     <row r="2006" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -30292,7 +30343,7 @@
         <v>2014</v>
       </c>
       <c r="B2016" s="1" t="s">
-        <v>4476</v>
+        <v>4473</v>
       </c>
     </row>
     <row r="2017" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -30380,7 +30431,7 @@
         <v>2025</v>
       </c>
       <c r="B2027" s="1" t="s">
-        <v>4477</v>
+        <v>4474</v>
       </c>
     </row>
     <row r="2028" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -30460,7 +30511,7 @@
         <v>2035</v>
       </c>
       <c r="B2037" s="1" t="s">
-        <v>4478</v>
+        <v>4475</v>
       </c>
     </row>
     <row r="2038" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -30551,12 +30602,12 @@
         <v>2046</v>
       </c>
     </row>
-    <row r="2049" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2049" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A2049" s="1" t="s">
         <v>2047</v>
       </c>
       <c r="B2049" s="1" t="s">
-        <v>2047</v>
+        <v>4476</v>
       </c>
     </row>
     <row r="2050" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -30639,12 +30690,12 @@
         <v>2057</v>
       </c>
     </row>
-    <row r="2060" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2060" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A2060" s="1" t="s">
         <v>2058</v>
       </c>
       <c r="B2060" s="1" t="s">
-        <v>2058</v>
+        <v>4476</v>
       </c>
     </row>
     <row r="2061" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -30727,12 +30778,12 @@
         <v>2068</v>
       </c>
     </row>
-    <row r="2071" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2071" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A2071" s="1" t="s">
         <v>2069</v>
       </c>
       <c r="B2071" s="1" t="s">
-        <v>2069</v>
+        <v>4477</v>
       </c>
     </row>
     <row r="2072" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -30815,12 +30866,12 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="2082" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2082" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A2082" s="1" t="s">
         <v>2080</v>
       </c>
       <c r="B2082" s="1" t="s">
-        <v>2080</v>
+        <v>4477</v>
       </c>
     </row>
     <row r="2083" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -30903,12 +30954,12 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="2093" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2093" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2093" s="1" t="s">
         <v>2091</v>
       </c>
       <c r="B2093" s="1" t="s">
-        <v>2091</v>
+        <v>4478</v>
       </c>
     </row>
     <row r="2094" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -31343,12 +31394,12 @@
         <v>2145</v>
       </c>
     </row>
-    <row r="2148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2148" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2148" s="1" t="s">
         <v>2146</v>
       </c>
       <c r="B2148" s="1" t="s">
-        <v>2146</v>
+        <v>4479</v>
       </c>
     </row>
     <row r="2149" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -31439,12 +31490,12 @@
         <v>2157</v>
       </c>
     </row>
-    <row r="2160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2160" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2160" s="1" t="s">
         <v>2158</v>
       </c>
       <c r="B2160" s="1" t="s">
-        <v>2158</v>
+        <v>4480</v>
       </c>
     </row>
     <row r="2161" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -31519,12 +31570,12 @@
         <v>2167</v>
       </c>
     </row>
-    <row r="2170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2170" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A2170" s="1" t="s">
         <v>2168</v>
       </c>
       <c r="B2170" s="1" t="s">
-        <v>2168</v>
+        <v>4481</v>
       </c>
     </row>
     <row r="2171" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -31615,12 +31666,12 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="2182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2182" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A2182" s="1" t="s">
         <v>2180</v>
       </c>
       <c r="B2182" s="1" t="s">
-        <v>2180</v>
+        <v>4481</v>
       </c>
     </row>
     <row r="2183" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -31703,12 +31754,12 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="2193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2193" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2193" s="1" t="s">
         <v>2191</v>
       </c>
       <c r="B2193" s="1" t="s">
-        <v>2191</v>
+        <v>4482</v>
       </c>
     </row>
     <row r="2194" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -31783,12 +31834,12 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="2203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2203" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A2203" s="1" t="s">
         <v>2201</v>
       </c>
       <c r="B2203" s="1" t="s">
-        <v>2201</v>
+        <v>4483</v>
       </c>
     </row>
     <row r="2204" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -31879,7 +31930,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="2215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2215" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2215" s="1" t="s">
         <v>2213</v>
       </c>
@@ -32055,15 +32106,15 @@
         <v>2234</v>
       </c>
     </row>
-    <row r="2237" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2237" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2237" s="1" t="s">
         <v>2235</v>
       </c>
       <c r="B2237" s="1" t="s">
-        <v>2235</v>
-      </c>
-    </row>
-    <row r="2238" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4484</v>
+      </c>
+    </row>
+    <row r="2238" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2238" s="1" t="s">
         <v>2236</v>
       </c>
@@ -32151,7 +32202,7 @@
         <v>2246</v>
       </c>
     </row>
-    <row r="2249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2249" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2249" s="1" t="s">
         <v>2247</v>
       </c>
@@ -32273,194 +32324,194 @@
     </row>
     <row r="2264" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2264" s="1" t="s">
-        <v>2262</v>
+        <v>3570</v>
       </c>
       <c r="B2264" s="1" t="s">
-        <v>2262</v>
+        <v>3570</v>
       </c>
     </row>
     <row r="2265" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2265" s="1" t="s">
-        <v>2263</v>
+        <v>3571</v>
       </c>
       <c r="B2265" s="1" t="s">
-        <v>2263</v>
+        <v>3571</v>
       </c>
     </row>
     <row r="2266" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2266" s="1" t="s">
-        <v>3573</v>
+        <v>3572</v>
       </c>
       <c r="B2266" s="1" t="s">
-        <v>3573</v>
+        <v>3572</v>
       </c>
     </row>
     <row r="2267" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2267" s="1" t="s">
-        <v>3574</v>
+        <v>3573</v>
       </c>
       <c r="B2267" s="1" t="s">
-        <v>3574</v>
+        <v>3573</v>
       </c>
     </row>
     <row r="2268" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2268" s="1" t="s">
-        <v>3575</v>
+        <v>3574</v>
       </c>
       <c r="B2268" s="1" t="s">
-        <v>3575</v>
+        <v>3574</v>
       </c>
     </row>
     <row r="2269" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2269" s="1" t="s">
+        <v>3575</v>
+      </c>
+      <c r="B2269" s="1" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="2270" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2270" s="1" t="s">
         <v>3576</v>
       </c>
-      <c r="B2269" s="1" t="s">
-        <v>3576</v>
-      </c>
-    </row>
-    <row r="2270" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2270" s="1" t="s">
-        <v>3577</v>
-      </c>
       <c r="B2270" s="1" t="s">
-        <v>3577</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="2271" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2271" s="1" t="s">
+        <v>3577</v>
+      </c>
+      <c r="B2271" s="1" t="s">
+        <v>3577</v>
+      </c>
+    </row>
+    <row r="2272" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2272" s="1" t="s">
         <v>3578</v>
       </c>
-      <c r="B2271" s="1" t="s">
+      <c r="B2272" s="1" t="s">
         <v>3578</v>
-      </c>
-    </row>
-    <row r="2272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2272" s="1" t="s">
-        <v>3579</v>
-      </c>
-      <c r="B2272" s="1" t="s">
-        <v>3579</v>
       </c>
     </row>
     <row r="2273" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2273" s="1" t="s">
-        <v>3580</v>
+        <v>3579</v>
       </c>
       <c r="B2273" s="1" t="s">
-        <v>3580</v>
+        <v>3579</v>
       </c>
     </row>
     <row r="2274" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2274" s="1" t="s">
-        <v>3581</v>
+        <v>3580</v>
       </c>
       <c r="B2274" s="1" t="s">
-        <v>3581</v>
+        <v>3580</v>
       </c>
     </row>
     <row r="2275" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2275" s="1" t="s">
-        <v>3582</v>
+        <v>3581</v>
       </c>
       <c r="B2275" s="1" t="s">
-        <v>3582</v>
+        <v>3581</v>
       </c>
     </row>
     <row r="2276" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2276" s="1" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
       <c r="B2276" s="1" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
     </row>
     <row r="2277" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2277" s="1" t="s">
-        <v>3584</v>
+        <v>3583</v>
       </c>
       <c r="B2277" s="1" t="s">
-        <v>3584</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="2278" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2278" s="1" t="s">
-        <v>3585</v>
+        <v>3584</v>
       </c>
       <c r="B2278" s="1" t="s">
-        <v>3585</v>
+        <v>3584</v>
       </c>
     </row>
     <row r="2279" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2279" s="1" t="s">
+        <v>3585</v>
+      </c>
+      <c r="B2279" s="1" t="s">
+        <v>3585</v>
+      </c>
+    </row>
+    <row r="2280" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2280" s="1" t="s">
         <v>3586</v>
       </c>
-      <c r="B2279" s="1" t="s">
-        <v>3586</v>
-      </c>
-    </row>
-    <row r="2280" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2280" s="1" t="s">
-        <v>3587</v>
-      </c>
       <c r="B2280" s="1" t="s">
-        <v>3587</v>
+        <v>4486</v>
       </c>
     </row>
     <row r="2281" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2281" s="1" t="s">
+        <v>3587</v>
+      </c>
+      <c r="B2281" s="1" t="s">
+        <v>3587</v>
+      </c>
+    </row>
+    <row r="2282" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2282" s="1" t="s">
         <v>3588</v>
       </c>
-      <c r="B2281" s="1" t="s">
+      <c r="B2282" s="1" t="s">
         <v>3588</v>
-      </c>
-    </row>
-    <row r="2282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2282" s="1" t="s">
-        <v>3589</v>
-      </c>
-      <c r="B2282" s="1" t="s">
-        <v>3589</v>
       </c>
     </row>
     <row r="2283" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2283" s="1" t="s">
-        <v>3590</v>
+        <v>3589</v>
       </c>
       <c r="B2283" s="1" t="s">
-        <v>3590</v>
+        <v>3589</v>
       </c>
     </row>
     <row r="2284" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2284" s="1" t="s">
-        <v>3591</v>
+        <v>3590</v>
       </c>
       <c r="B2284" s="1" t="s">
-        <v>3591</v>
+        <v>3590</v>
       </c>
     </row>
     <row r="2285" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2285" s="1" t="s">
-        <v>3592</v>
+        <v>3591</v>
       </c>
       <c r="B2285" s="1" t="s">
-        <v>3592</v>
+        <v>3591</v>
       </c>
     </row>
     <row r="2286" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2286" s="1" t="s">
-        <v>3593</v>
+        <v>2284</v>
       </c>
       <c r="B2286" s="1" t="s">
-        <v>3593</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="2287" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2287" s="1" t="s">
-        <v>3594</v>
+        <v>2285</v>
       </c>
       <c r="B2287" s="1" t="s">
-        <v>3594</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="2288" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -32495,12 +32546,12 @@
         <v>2289</v>
       </c>
     </row>
-    <row r="2292" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2292" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2292" s="1" t="s">
         <v>2290</v>
       </c>
       <c r="B2292" s="1" t="s">
-        <v>2290</v>
+        <v>4487</v>
       </c>
     </row>
     <row r="2293" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -32511,7 +32562,7 @@
         <v>2291</v>
       </c>
     </row>
-    <row r="2294" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2294" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2294" s="1" t="s">
         <v>2292</v>
       </c>
@@ -32537,18 +32588,18 @@
     </row>
     <row r="2297" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2297" s="1" t="s">
-        <v>2295</v>
+        <v>2273</v>
       </c>
       <c r="B2297" s="1" t="s">
-        <v>2295</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="2298" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2298" s="1" t="s">
-        <v>2296</v>
+        <v>2274</v>
       </c>
       <c r="B2298" s="1" t="s">
-        <v>2296</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="2299" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -32583,12 +32634,12 @@
         <v>2278</v>
       </c>
     </row>
-    <row r="2303" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2303" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2303" s="1" t="s">
         <v>2279</v>
       </c>
       <c r="B2303" s="1" t="s">
-        <v>2279</v>
+        <v>4489</v>
       </c>
     </row>
     <row r="2304" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -32599,7 +32650,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="2305" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2305" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2305" s="1" t="s">
         <v>2281</v>
       </c>
@@ -32625,722 +32676,722 @@
     </row>
     <row r="2308" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2308" s="1" t="s">
-        <v>2284</v>
+        <v>3592</v>
       </c>
       <c r="B2308" s="1" t="s">
-        <v>2284</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="2309" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2309" s="1" t="s">
-        <v>2285</v>
+        <v>3593</v>
       </c>
       <c r="B2309" s="1" t="s">
-        <v>2285</v>
+        <v>3593</v>
       </c>
     </row>
     <row r="2310" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2310" s="1" t="s">
-        <v>3595</v>
+        <v>3594</v>
       </c>
       <c r="B2310" s="1" t="s">
-        <v>3595</v>
+        <v>3594</v>
       </c>
     </row>
     <row r="2311" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2311" s="1" t="s">
-        <v>3596</v>
+        <v>3595</v>
       </c>
       <c r="B2311" s="1" t="s">
-        <v>3596</v>
+        <v>3595</v>
       </c>
     </row>
     <row r="2312" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2312" s="1" t="s">
-        <v>3597</v>
+        <v>3596</v>
       </c>
       <c r="B2312" s="1" t="s">
-        <v>3597</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="2313" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2313" s="1" t="s">
-        <v>3598</v>
+        <v>3597</v>
       </c>
       <c r="B2313" s="1" t="s">
-        <v>3598</v>
+        <v>3597</v>
       </c>
     </row>
     <row r="2314" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2314" s="1" t="s">
-        <v>3599</v>
+        <v>3598</v>
       </c>
       <c r="B2314" s="1" t="s">
-        <v>3599</v>
+        <v>3598</v>
       </c>
     </row>
     <row r="2315" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2315" s="1" t="s">
-        <v>3600</v>
+        <v>3599</v>
       </c>
       <c r="B2315" s="1" t="s">
-        <v>3600</v>
+        <v>3599</v>
       </c>
     </row>
     <row r="2316" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2316" s="1" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
       <c r="B2316" s="1" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="2317" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2317" s="1" t="s">
-        <v>3602</v>
+        <v>3601</v>
       </c>
       <c r="B2317" s="1" t="s">
-        <v>3602</v>
+        <v>3601</v>
       </c>
     </row>
     <row r="2318" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2318" s="1" t="s">
-        <v>3603</v>
+        <v>3602</v>
       </c>
       <c r="B2318" s="1" t="s">
-        <v>3603</v>
+        <v>3602</v>
       </c>
     </row>
     <row r="2319" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2319" s="1" t="s">
-        <v>3604</v>
+        <v>3603</v>
       </c>
       <c r="B2319" s="1" t="s">
-        <v>3604</v>
+        <v>3603</v>
       </c>
     </row>
     <row r="2320" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2320" s="1" t="s">
-        <v>3605</v>
+        <v>3604</v>
       </c>
       <c r="B2320" s="1" t="s">
-        <v>3605</v>
+        <v>3604</v>
       </c>
     </row>
     <row r="2321" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2321" s="1" t="s">
-        <v>3606</v>
+        <v>3605</v>
       </c>
       <c r="B2321" s="1" t="s">
-        <v>3606</v>
+        <v>3605</v>
       </c>
     </row>
     <row r="2322" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2322" s="1" t="s">
-        <v>3607</v>
+        <v>3606</v>
       </c>
       <c r="B2322" s="1" t="s">
-        <v>3607</v>
+        <v>3606</v>
       </c>
     </row>
     <row r="2323" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2323" s="1" t="s">
+        <v>3607</v>
+      </c>
+      <c r="B2323" s="1" t="s">
+        <v>3607</v>
+      </c>
+    </row>
+    <row r="2324" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2324" s="1" t="s">
         <v>3608</v>
       </c>
-      <c r="B2323" s="1" t="s">
-        <v>3608</v>
-      </c>
-    </row>
-    <row r="2324" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2324" s="1" t="s">
-        <v>3609</v>
-      </c>
       <c r="B2324" s="1" t="s">
-        <v>3609</v>
+        <v>4488</v>
       </c>
     </row>
     <row r="2325" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2325" s="1" t="s">
+        <v>3609</v>
+      </c>
+      <c r="B2325" s="1" t="s">
+        <v>3609</v>
+      </c>
+    </row>
+    <row r="2326" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2326" s="1" t="s">
         <v>3610</v>
       </c>
-      <c r="B2325" s="1" t="s">
+      <c r="B2326" s="1" t="s">
         <v>3610</v>
-      </c>
-    </row>
-    <row r="2326" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2326" s="1" t="s">
-        <v>3611</v>
-      </c>
-      <c r="B2326" s="1" t="s">
-        <v>3611</v>
       </c>
     </row>
     <row r="2327" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2327" s="1" t="s">
-        <v>3612</v>
+        <v>3611</v>
       </c>
       <c r="B2327" s="1" t="s">
-        <v>3612</v>
+        <v>3611</v>
       </c>
     </row>
     <row r="2328" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2328" s="1" t="s">
-        <v>3613</v>
+        <v>3612</v>
       </c>
       <c r="B2328" s="1" t="s">
-        <v>3613</v>
+        <v>3612</v>
       </c>
     </row>
     <row r="2329" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2329" s="1" t="s">
-        <v>3614</v>
+        <v>3613</v>
       </c>
       <c r="B2329" s="1" t="s">
-        <v>3614</v>
+        <v>3613</v>
       </c>
     </row>
     <row r="2330" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2330" s="1" t="s">
-        <v>3615</v>
+        <v>3614</v>
       </c>
       <c r="B2330" s="1" t="s">
-        <v>3615</v>
+        <v>3614</v>
       </c>
     </row>
     <row r="2331" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2331" s="1" t="s">
-        <v>3616</v>
+        <v>3615</v>
       </c>
       <c r="B2331" s="1" t="s">
-        <v>3616</v>
+        <v>3615</v>
       </c>
     </row>
     <row r="2332" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2332" s="1" t="s">
-        <v>3617</v>
+        <v>3616</v>
       </c>
       <c r="B2332" s="1" t="s">
-        <v>3617</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="2333" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2333" s="1" t="s">
-        <v>3618</v>
+        <v>3617</v>
       </c>
       <c r="B2333" s="1" t="s">
-        <v>3618</v>
+        <v>3617</v>
       </c>
     </row>
     <row r="2334" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2334" s="1" t="s">
+        <v>3618</v>
+      </c>
+      <c r="B2334" s="1" t="s">
+        <v>3618</v>
+      </c>
+    </row>
+    <row r="2335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2335" s="1" t="s">
         <v>3619</v>
       </c>
-      <c r="B2334" s="1" t="s">
-        <v>3619</v>
-      </c>
-    </row>
-    <row r="2335" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2335" s="1" t="s">
-        <v>3620</v>
-      </c>
       <c r="B2335" s="1" t="s">
-        <v>3620</v>
+        <v>4490</v>
       </c>
     </row>
     <row r="2336" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2336" s="1" t="s">
+        <v>3620</v>
+      </c>
+      <c r="B2336" s="1" t="s">
+        <v>3620</v>
+      </c>
+    </row>
+    <row r="2337" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2337" s="1" t="s">
         <v>3621</v>
       </c>
-      <c r="B2336" s="1" t="s">
+      <c r="B2337" s="1" t="s">
         <v>3621</v>
-      </c>
-    </row>
-    <row r="2337" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2337" s="1" t="s">
-        <v>3622</v>
-      </c>
-      <c r="B2337" s="1" t="s">
-        <v>3622</v>
       </c>
     </row>
     <row r="2338" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2338" s="1" t="s">
-        <v>3623</v>
+        <v>3622</v>
       </c>
       <c r="B2338" s="1" t="s">
-        <v>3623</v>
+        <v>3622</v>
       </c>
     </row>
     <row r="2339" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2339" s="1" t="s">
-        <v>3624</v>
+        <v>3623</v>
       </c>
       <c r="B2339" s="1" t="s">
-        <v>3624</v>
+        <v>3623</v>
       </c>
     </row>
     <row r="2340" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2340" s="1" t="s">
-        <v>3625</v>
+        <v>3624</v>
       </c>
       <c r="B2340" s="1" t="s">
-        <v>3625</v>
+        <v>3624</v>
       </c>
     </row>
     <row r="2341" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2341" s="1" t="s">
-        <v>3626</v>
+        <v>3625</v>
       </c>
       <c r="B2341" s="1" t="s">
-        <v>3626</v>
+        <v>3625</v>
       </c>
     </row>
     <row r="2342" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2342" s="1" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
       <c r="B2342" s="1" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
     </row>
     <row r="2343" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2343" s="1" t="s">
-        <v>3628</v>
+        <v>3627</v>
       </c>
       <c r="B2343" s="1" t="s">
-        <v>3628</v>
+        <v>3627</v>
       </c>
     </row>
     <row r="2344" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2344" s="1" t="s">
-        <v>3629</v>
+        <v>3628</v>
       </c>
       <c r="B2344" s="1" t="s">
-        <v>3629</v>
+        <v>3628</v>
       </c>
     </row>
     <row r="2345" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2345" s="1" t="s">
-        <v>3630</v>
+        <v>3629</v>
       </c>
       <c r="B2345" s="1" t="s">
-        <v>3630</v>
+        <v>3629</v>
       </c>
     </row>
     <row r="2346" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2346" s="1" t="s">
+        <v>3630</v>
+      </c>
+      <c r="B2346" s="1" t="s">
+        <v>3630</v>
+      </c>
+    </row>
+    <row r="2347" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2347" s="1" t="s">
         <v>3631</v>
       </c>
-      <c r="B2346" s="1" t="s">
-        <v>3631</v>
-      </c>
-    </row>
-    <row r="2347" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2347" s="1" t="s">
-        <v>3632</v>
-      </c>
       <c r="B2347" s="1" t="s">
-        <v>3632</v>
+        <v>4491</v>
       </c>
     </row>
     <row r="2348" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2348" s="1" t="s">
+        <v>3632</v>
+      </c>
+      <c r="B2348" s="1" t="s">
+        <v>3632</v>
+      </c>
+    </row>
+    <row r="2349" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2349" s="1" t="s">
         <v>3633</v>
       </c>
-      <c r="B2348" s="1" t="s">
+      <c r="B2349" s="1" t="s">
         <v>3633</v>
-      </c>
-    </row>
-    <row r="2349" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2349" s="1" t="s">
-        <v>3634</v>
-      </c>
-      <c r="B2349" s="1" t="s">
-        <v>3634</v>
       </c>
     </row>
     <row r="2350" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2350" s="1" t="s">
-        <v>3635</v>
+        <v>3634</v>
       </c>
       <c r="B2350" s="1" t="s">
-        <v>3635</v>
+        <v>3634</v>
       </c>
     </row>
     <row r="2351" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2351" s="1" t="s">
-        <v>3636</v>
+        <v>3635</v>
       </c>
       <c r="B2351" s="1" t="s">
-        <v>3636</v>
+        <v>3635</v>
       </c>
     </row>
     <row r="2352" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2352" s="1" t="s">
-        <v>3637</v>
+        <v>3636</v>
       </c>
       <c r="B2352" s="1" t="s">
-        <v>3637</v>
+        <v>3636</v>
       </c>
     </row>
     <row r="2353" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2353" s="1" t="s">
-        <v>3638</v>
+        <v>3637</v>
       </c>
       <c r="B2353" s="1" t="s">
-        <v>3638</v>
+        <v>3637</v>
       </c>
     </row>
     <row r="2354" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2354" s="1" t="s">
-        <v>3639</v>
+        <v>3638</v>
       </c>
       <c r="B2354" s="1" t="s">
-        <v>3639</v>
+        <v>3638</v>
       </c>
     </row>
     <row r="2355" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2355" s="1" t="s">
-        <v>3640</v>
+        <v>3639</v>
       </c>
       <c r="B2355" s="1" t="s">
-        <v>3640</v>
+        <v>3639</v>
       </c>
     </row>
     <row r="2356" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2356" s="1" t="s">
-        <v>3641</v>
+        <v>3640</v>
       </c>
       <c r="B2356" s="1" t="s">
-        <v>3641</v>
+        <v>3640</v>
       </c>
     </row>
     <row r="2357" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2357" s="1" t="s">
+        <v>3641</v>
+      </c>
+      <c r="B2357" s="1" t="s">
+        <v>3641</v>
+      </c>
+    </row>
+    <row r="2358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2358" s="1" t="s">
         <v>3642</v>
       </c>
-      <c r="B2357" s="1" t="s">
-        <v>3642</v>
-      </c>
-    </row>
-    <row r="2358" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2358" s="1" t="s">
-        <v>3643</v>
-      </c>
       <c r="B2358" s="1" t="s">
-        <v>3643</v>
+        <v>4492</v>
       </c>
     </row>
     <row r="2359" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2359" s="1" t="s">
+        <v>3643</v>
+      </c>
+      <c r="B2359" s="1" t="s">
+        <v>3643</v>
+      </c>
+    </row>
+    <row r="2360" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2360" s="1" t="s">
         <v>3644</v>
       </c>
-      <c r="B2359" s="1" t="s">
+      <c r="B2360" s="1" t="s">
         <v>3644</v>
-      </c>
-    </row>
-    <row r="2360" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2360" s="1" t="s">
-        <v>3645</v>
-      </c>
-      <c r="B2360" s="1" t="s">
-        <v>3645</v>
       </c>
     </row>
     <row r="2361" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2361" s="1" t="s">
-        <v>3646</v>
+        <v>3645</v>
       </c>
       <c r="B2361" s="1" t="s">
-        <v>3646</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="2362" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2362" s="1" t="s">
-        <v>3647</v>
+        <v>3646</v>
       </c>
       <c r="B2362" s="1" t="s">
-        <v>3647</v>
+        <v>3646</v>
       </c>
     </row>
     <row r="2363" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2363" s="1" t="s">
-        <v>3648</v>
+        <v>3647</v>
       </c>
       <c r="B2363" s="1" t="s">
-        <v>3648</v>
+        <v>3647</v>
       </c>
     </row>
     <row r="2364" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2364" s="1" t="s">
-        <v>3649</v>
+        <v>3648</v>
       </c>
       <c r="B2364" s="1" t="s">
-        <v>3649</v>
+        <v>3648</v>
       </c>
     </row>
     <row r="2365" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2365" s="1" t="s">
-        <v>3650</v>
+        <v>3649</v>
       </c>
       <c r="B2365" s="1" t="s">
-        <v>3650</v>
+        <v>3649</v>
       </c>
     </row>
     <row r="2366" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2366" s="1" t="s">
-        <v>3651</v>
+        <v>3650</v>
       </c>
       <c r="B2366" s="1" t="s">
-        <v>3651</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="2367" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2367" s="1" t="s">
-        <v>3652</v>
+        <v>3651</v>
       </c>
       <c r="B2367" s="1" t="s">
-        <v>3652</v>
+        <v>3651</v>
       </c>
     </row>
     <row r="2368" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2368" s="1" t="s">
-        <v>3653</v>
+        <v>3652</v>
       </c>
       <c r="B2368" s="1" t="s">
-        <v>3653</v>
+        <v>3652</v>
       </c>
     </row>
     <row r="2369" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2369" s="1" t="s">
-        <v>3654</v>
+        <v>3653</v>
       </c>
       <c r="B2369" s="1" t="s">
-        <v>3654</v>
+        <v>3653</v>
       </c>
     </row>
     <row r="2370" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2370" s="1" t="s">
-        <v>3655</v>
+        <v>3654</v>
       </c>
       <c r="B2370" s="1" t="s">
-        <v>3655</v>
+        <v>3654</v>
       </c>
     </row>
     <row r="2371" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2371" s="1" t="s">
-        <v>3656</v>
+        <v>3655</v>
       </c>
       <c r="B2371" s="1" t="s">
-        <v>3656</v>
+        <v>3655</v>
       </c>
     </row>
     <row r="2372" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2372" s="1" t="s">
-        <v>3657</v>
+        <v>3656</v>
       </c>
       <c r="B2372" s="1" t="s">
-        <v>3657</v>
+        <v>3656</v>
       </c>
     </row>
     <row r="2373" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2373" s="1" t="s">
-        <v>3658</v>
+        <v>3657</v>
       </c>
       <c r="B2373" s="1" t="s">
-        <v>3658</v>
+        <v>3657</v>
       </c>
     </row>
     <row r="2374" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2374" s="1" t="s">
-        <v>3659</v>
+        <v>3658</v>
       </c>
       <c r="B2374" s="1" t="s">
-        <v>3659</v>
+        <v>3658</v>
       </c>
     </row>
     <row r="2375" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2375" s="1" t="s">
-        <v>3660</v>
+        <v>3659</v>
       </c>
       <c r="B2375" s="1" t="s">
-        <v>3660</v>
+        <v>3659</v>
       </c>
     </row>
     <row r="2376" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2376" s="1" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
       <c r="B2376" s="1" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
     </row>
     <row r="2377" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2377" s="1" t="s">
-        <v>3662</v>
+        <v>3661</v>
       </c>
       <c r="B2377" s="1" t="s">
-        <v>3662</v>
+        <v>3661</v>
       </c>
     </row>
     <row r="2378" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2378" s="1" t="s">
+        <v>3662</v>
+      </c>
+      <c r="B2378" s="1" t="s">
+        <v>3662</v>
+      </c>
+    </row>
+    <row r="2379" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2379" s="1" t="s">
         <v>3663</v>
       </c>
-      <c r="B2378" s="1" t="s">
-        <v>3663</v>
-      </c>
-    </row>
-    <row r="2379" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2379" s="1" t="s">
-        <v>3664</v>
-      </c>
       <c r="B2379" s="1" t="s">
-        <v>3664</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="2380" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2380" s="1" t="s">
+        <v>3664</v>
+      </c>
+      <c r="B2380" s="1" t="s">
+        <v>3664</v>
+      </c>
+    </row>
+    <row r="2381" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2381" s="1" t="s">
         <v>3665</v>
       </c>
-      <c r="B2380" s="1" t="s">
+      <c r="B2381" s="1" t="s">
         <v>3665</v>
-      </c>
-    </row>
-    <row r="2381" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2381" s="1" t="s">
-        <v>3666</v>
-      </c>
-      <c r="B2381" s="1" t="s">
-        <v>3666</v>
       </c>
     </row>
     <row r="2382" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2382" s="1" t="s">
-        <v>3667</v>
+        <v>3666</v>
       </c>
       <c r="B2382" s="1" t="s">
-        <v>3667</v>
+        <v>3666</v>
       </c>
     </row>
     <row r="2383" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2383" s="1" t="s">
-        <v>3668</v>
+        <v>3667</v>
       </c>
       <c r="B2383" s="1" t="s">
-        <v>3668</v>
+        <v>3667</v>
       </c>
     </row>
     <row r="2384" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2384" s="1" t="s">
-        <v>3669</v>
+        <v>3668</v>
       </c>
       <c r="B2384" s="1" t="s">
-        <v>3669</v>
+        <v>3668</v>
       </c>
     </row>
     <row r="2385" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2385" s="1" t="s">
-        <v>3670</v>
+        <v>3669</v>
       </c>
       <c r="B2385" s="1" t="s">
-        <v>3670</v>
+        <v>3669</v>
       </c>
     </row>
     <row r="2386" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2386" s="1" t="s">
-        <v>3671</v>
+        <v>3670</v>
       </c>
       <c r="B2386" s="1" t="s">
-        <v>3671</v>
+        <v>3670</v>
       </c>
     </row>
     <row r="2387" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2387" s="1" t="s">
-        <v>3672</v>
+        <v>3671</v>
       </c>
       <c r="B2387" s="1" t="s">
-        <v>3672</v>
+        <v>3671</v>
       </c>
     </row>
     <row r="2388" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2388" s="1" t="s">
-        <v>3673</v>
+        <v>3672</v>
       </c>
       <c r="B2388" s="1" t="s">
-        <v>3673</v>
+        <v>3672</v>
       </c>
     </row>
     <row r="2389" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2389" s="1" t="s">
+        <v>3673</v>
+      </c>
+      <c r="B2389" s="1" t="s">
+        <v>3673</v>
+      </c>
+    </row>
+    <row r="2390" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2390" s="1" t="s">
         <v>3674</v>
       </c>
-      <c r="B2389" s="1" t="s">
-        <v>3674</v>
-      </c>
-    </row>
-    <row r="2390" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2390" s="1" t="s">
-        <v>3675</v>
-      </c>
       <c r="B2390" s="1" t="s">
-        <v>3675</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="2391" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2391" s="1" t="s">
+        <v>3675</v>
+      </c>
+      <c r="B2391" s="1" t="s">
+        <v>3675</v>
+      </c>
+    </row>
+    <row r="2392" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2392" s="1" t="s">
         <v>3676</v>
       </c>
-      <c r="B2391" s="1" t="s">
+      <c r="B2392" s="1" t="s">
         <v>3676</v>
-      </c>
-    </row>
-    <row r="2392" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2392" s="1" t="s">
-        <v>3677</v>
-      </c>
-      <c r="B2392" s="1" t="s">
-        <v>3677</v>
       </c>
     </row>
     <row r="2393" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2393" s="1" t="s">
-        <v>3678</v>
+        <v>3677</v>
       </c>
       <c r="B2393" s="1" t="s">
-        <v>3678</v>
+        <v>3677</v>
       </c>
     </row>
     <row r="2394" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2394" s="1" t="s">
-        <v>3679</v>
+        <v>3678</v>
       </c>
       <c r="B2394" s="1" t="s">
-        <v>3679</v>
+        <v>3678</v>
       </c>
     </row>
     <row r="2395" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2395" s="1" t="s">
-        <v>3680</v>
+        <v>3679</v>
       </c>
       <c r="B2395" s="1" t="s">
-        <v>3680</v>
+        <v>3679</v>
       </c>
     </row>
     <row r="2396" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2396" s="1" t="s">
-        <v>3681</v>
+        <v>2262</v>
       </c>
       <c r="B2396" s="1" t="s">
-        <v>3681</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="2397" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2397" s="1" t="s">
-        <v>3682</v>
+        <v>2263</v>
       </c>
       <c r="B2397" s="1" t="s">
-        <v>3682</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="2398" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33375,12 +33426,12 @@
         <v>2267</v>
       </c>
     </row>
-    <row r="2402" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2402" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2402" s="1" t="s">
         <v>2268</v>
       </c>
       <c r="B2402" s="1" t="s">
-        <v>2268</v>
+        <v>4495</v>
       </c>
     </row>
     <row r="2403" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33391,7 +33442,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="2404" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2404" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2404" s="1" t="s">
         <v>2270</v>
       </c>
@@ -33417,18 +33468,18 @@
     </row>
     <row r="2407" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2407" s="1" t="s">
-        <v>2273</v>
+        <v>2295</v>
       </c>
       <c r="B2407" s="1" t="s">
-        <v>2273</v>
+        <v>2295</v>
       </c>
     </row>
     <row r="2408" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2408" s="1" t="s">
-        <v>2274</v>
+        <v>2296</v>
       </c>
       <c r="B2408" s="1" t="s">
-        <v>2274</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="2409" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33479,7 +33530,7 @@
         <v>2302</v>
       </c>
     </row>
-    <row r="2415" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2415" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2415" s="1" t="s">
         <v>2303</v>
       </c>
@@ -33505,26 +33556,26 @@
     </row>
     <row r="2418" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2418" s="1" t="s">
-        <v>2306</v>
+        <v>3680</v>
       </c>
       <c r="B2418" s="1" t="s">
-        <v>2306</v>
+        <v>3680</v>
       </c>
     </row>
     <row r="2419" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2419" s="1" t="s">
-        <v>2307</v>
+        <v>3681</v>
       </c>
       <c r="B2419" s="1" t="s">
-        <v>2307</v>
+        <v>3681</v>
       </c>
     </row>
     <row r="2420" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2420" s="1" t="s">
-        <v>2308</v>
+        <v>3682</v>
       </c>
       <c r="B2420" s="1" t="s">
-        <v>2308</v>
+        <v>3682</v>
       </c>
     </row>
     <row r="2421" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33543,12 +33594,12 @@
         <v>3684</v>
       </c>
     </row>
-    <row r="2423" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2423" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2423" s="1" t="s">
         <v>3685</v>
       </c>
       <c r="B2423" s="1" t="s">
-        <v>3685</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="2424" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33567,7 +33618,7 @@
         <v>3687</v>
       </c>
     </row>
-    <row r="2426" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2426" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2426" s="1" t="s">
         <v>3688</v>
       </c>
@@ -33593,26 +33644,26 @@
     </row>
     <row r="2429" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2429" s="1" t="s">
-        <v>3691</v>
+        <v>2306</v>
       </c>
       <c r="B2429" s="1" t="s">
-        <v>3691</v>
+        <v>4359</v>
       </c>
     </row>
     <row r="2430" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2430" s="1" t="s">
-        <v>3692</v>
+        <v>2307</v>
       </c>
       <c r="B2430" s="1" t="s">
-        <v>3692</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="2431" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2431" s="1" t="s">
-        <v>3693</v>
+        <v>2308</v>
       </c>
       <c r="B2431" s="1" t="s">
-        <v>3693</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="2432" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33620,7 +33671,7 @@
         <v>2309</v>
       </c>
       <c r="B2432" s="1" t="s">
-        <v>4362</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="2433" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33639,12 +33690,12 @@
         <v>2311</v>
       </c>
     </row>
-    <row r="2435" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2435" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2435" s="1" t="s">
         <v>2312</v>
       </c>
       <c r="B2435" s="1" t="s">
-        <v>2312</v>
+        <v>4357</v>
       </c>
     </row>
     <row r="2436" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33663,12 +33714,12 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="2438" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2438" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2438" s="1" t="s">
         <v>2315</v>
       </c>
       <c r="B2438" s="1" t="s">
-        <v>4360</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="2439" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33692,7 +33743,7 @@
         <v>2318</v>
       </c>
       <c r="B2441" s="1" t="s">
-        <v>2318</v>
+        <v>4403</v>
       </c>
     </row>
     <row r="2442" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33700,7 +33751,7 @@
         <v>2319</v>
       </c>
       <c r="B2442" s="1" t="s">
-        <v>2319</v>
+        <v>4403</v>
       </c>
     </row>
     <row r="2443" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33716,7 +33767,7 @@
         <v>2321</v>
       </c>
       <c r="B2444" s="1" t="s">
-        <v>4406</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="2445" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33724,55 +33775,55 @@
         <v>2322</v>
       </c>
       <c r="B2445" s="1" t="s">
-        <v>4406</v>
-      </c>
-    </row>
-    <row r="2446" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>2322</v>
+      </c>
+    </row>
+    <row r="2446" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2446" s="1" t="s">
         <v>2323</v>
       </c>
       <c r="B2446" s="1" t="s">
-        <v>2323</v>
-      </c>
-    </row>
-    <row r="2447" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4402</v>
+      </c>
+    </row>
+    <row r="2447" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2447" s="1" t="s">
         <v>2324</v>
       </c>
       <c r="B2447" s="1" t="s">
-        <v>2324</v>
-      </c>
-    </row>
-    <row r="2448" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4402</v>
+      </c>
+    </row>
+    <row r="2448" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2448" s="1" t="s">
         <v>2325</v>
       </c>
       <c r="B2448" s="1" t="s">
-        <v>2325</v>
-      </c>
-    </row>
-    <row r="2449" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>4402</v>
+      </c>
+    </row>
+    <row r="2449" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2449" s="1" t="s">
         <v>2326</v>
       </c>
       <c r="B2449" s="1" t="s">
-        <v>4405</v>
-      </c>
-    </row>
-    <row r="2450" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>2326</v>
+      </c>
+    </row>
+    <row r="2450" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2450" s="1" t="s">
         <v>2327</v>
       </c>
       <c r="B2450" s="1" t="s">
-        <v>4405</v>
-      </c>
-    </row>
-    <row r="2451" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>2327</v>
+      </c>
+    </row>
+    <row r="2451" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2451" s="1" t="s">
         <v>2328</v>
       </c>
       <c r="B2451" s="1" t="s">
-        <v>4405</v>
+        <v>2328</v>
       </c>
     </row>
     <row r="2452" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33780,7 +33831,7 @@
         <v>2329</v>
       </c>
       <c r="B2452" s="1" t="s">
-        <v>2329</v>
+        <v>4403</v>
       </c>
     </row>
     <row r="2453" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33788,7 +33839,7 @@
         <v>2330</v>
       </c>
       <c r="B2453" s="1" t="s">
-        <v>2330</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="2454" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33804,7 +33855,7 @@
         <v>2332</v>
       </c>
       <c r="B2455" s="1" t="s">
-        <v>4406</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="2456" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33812,7 +33863,7 @@
         <v>2333</v>
       </c>
       <c r="B2456" s="1" t="s">
-        <v>4402</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="2457" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33916,7 +33967,7 @@
         <v>2346</v>
       </c>
       <c r="B2469" s="1" t="s">
-        <v>2346</v>
+        <v>4387</v>
       </c>
     </row>
     <row r="2470" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33940,7 +33991,7 @@
         <v>2349</v>
       </c>
       <c r="B2472" s="1" t="s">
-        <v>4390</v>
+        <v>2349</v>
       </c>
     </row>
     <row r="2473" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33964,7 +34015,7 @@
         <v>2352</v>
       </c>
       <c r="B2475" s="1" t="s">
-        <v>2352</v>
+        <v>4387</v>
       </c>
     </row>
     <row r="2476" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33988,7 +34039,7 @@
         <v>2355</v>
       </c>
       <c r="B2478" s="1" t="s">
-        <v>4390</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="2479" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -33999,12 +34050,12 @@
         <v>2356</v>
       </c>
     </row>
-    <row r="2480" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2480" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2480" s="1" t="s">
         <v>2357</v>
       </c>
       <c r="B2480" s="1" t="s">
-        <v>2357</v>
+        <v>4378</v>
       </c>
     </row>
     <row r="2481" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34012,7 +34063,7 @@
         <v>2358</v>
       </c>
       <c r="B2481" s="1" t="s">
-        <v>2358</v>
+        <v>4381</v>
       </c>
     </row>
     <row r="2482" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34020,15 +34071,15 @@
         <v>2359</v>
       </c>
       <c r="B2482" s="1" t="s">
-        <v>2359</v>
-      </c>
-    </row>
-    <row r="2483" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>4380</v>
+      </c>
+    </row>
+    <row r="2483" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2483" s="1" t="s">
         <v>2360</v>
       </c>
       <c r="B2483" s="1" t="s">
-        <v>4381</v>
+        <v>2360</v>
       </c>
     </row>
     <row r="2484" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34036,7 +34087,7 @@
         <v>2361</v>
       </c>
       <c r="B2484" s="1" t="s">
-        <v>4384</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="2485" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34044,15 +34095,15 @@
         <v>2362</v>
       </c>
       <c r="B2485" s="1" t="s">
-        <v>4383</v>
-      </c>
-    </row>
-    <row r="2486" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>2362</v>
+      </c>
+    </row>
+    <row r="2486" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2486" s="1" t="s">
         <v>2363</v>
       </c>
       <c r="B2486" s="1" t="s">
-        <v>2363</v>
+        <v>4379</v>
       </c>
     </row>
     <row r="2487" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34060,7 +34111,7 @@
         <v>2364</v>
       </c>
       <c r="B2487" s="1" t="s">
-        <v>2364</v>
+        <v>4381</v>
       </c>
     </row>
     <row r="2488" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34068,15 +34119,15 @@
         <v>2365</v>
       </c>
       <c r="B2488" s="1" t="s">
-        <v>2365</v>
-      </c>
-    </row>
-    <row r="2489" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>4380</v>
+      </c>
+    </row>
+    <row r="2489" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2489" s="1" t="s">
         <v>2366</v>
       </c>
       <c r="B2489" s="1" t="s">
-        <v>4382</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="2490" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34084,15 +34135,15 @@
         <v>2367</v>
       </c>
       <c r="B2490" s="1" t="s">
-        <v>4384</v>
-      </c>
-    </row>
-    <row r="2491" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>2367</v>
+      </c>
+    </row>
+    <row r="2491" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2491" s="1" t="s">
         <v>2368</v>
       </c>
       <c r="B2491" s="1" t="s">
-        <v>4383</v>
+        <v>4367</v>
       </c>
     </row>
     <row r="2492" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34111,12 +34162,12 @@
         <v>2370</v>
       </c>
     </row>
-    <row r="2494" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2494" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2494" s="1" t="s">
         <v>2371</v>
       </c>
       <c r="B2494" s="1" t="s">
-        <v>4370</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="2495" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34135,12 +34186,12 @@
         <v>2373</v>
       </c>
     </row>
-    <row r="2497" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2497" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2497" s="1" t="s">
         <v>2374</v>
       </c>
       <c r="B2497" s="1" t="s">
-        <v>2374</v>
+        <v>4367</v>
       </c>
     </row>
     <row r="2498" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34159,12 +34210,12 @@
         <v>2376</v>
       </c>
     </row>
-    <row r="2500" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2500" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2500" s="1" t="s">
         <v>2377</v>
       </c>
       <c r="B2500" s="1" t="s">
-        <v>4370</v>
+        <v>2377</v>
       </c>
     </row>
     <row r="2501" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34279,52 +34330,52 @@
         <v>2391</v>
       </c>
     </row>
-    <row r="2515" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2515" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2515" s="1" t="s">
         <v>2392</v>
       </c>
       <c r="B2515" s="1" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="2516" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4405</v>
+      </c>
+    </row>
+    <row r="2516" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2516" s="1" t="s">
         <v>2393</v>
       </c>
       <c r="B2516" s="1" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="2517" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4405</v>
+      </c>
+    </row>
+    <row r="2517" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2517" s="1" t="s">
         <v>2394</v>
       </c>
       <c r="B2517" s="1" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="2518" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>4405</v>
+      </c>
+    </row>
+    <row r="2518" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2518" s="1" t="s">
         <v>2395</v>
       </c>
       <c r="B2518" s="1" t="s">
-        <v>4408</v>
-      </c>
-    </row>
-    <row r="2519" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>2395</v>
+      </c>
+    </row>
+    <row r="2519" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2519" s="1" t="s">
         <v>2396</v>
       </c>
       <c r="B2519" s="1" t="s">
-        <v>4408</v>
-      </c>
-    </row>
-    <row r="2520" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>2396</v>
+      </c>
+    </row>
+    <row r="2520" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2520" s="1" t="s">
         <v>2397</v>
       </c>
       <c r="B2520" s="1" t="s">
-        <v>4408</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="2521" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34332,7 +34383,7 @@
         <v>2398</v>
       </c>
       <c r="B2521" s="1" t="s">
-        <v>2398</v>
+        <v>4404</v>
       </c>
     </row>
     <row r="2522" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34340,7 +34391,7 @@
         <v>2399</v>
       </c>
       <c r="B2522" s="1" t="s">
-        <v>2399</v>
+        <v>4404</v>
       </c>
     </row>
     <row r="2523" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34348,15 +34399,15 @@
         <v>2400</v>
       </c>
       <c r="B2523" s="1" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="2524" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4404</v>
+      </c>
+    </row>
+    <row r="2524" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2524" s="1" t="s">
         <v>2401</v>
       </c>
       <c r="B2524" s="1" t="s">
-        <v>4407</v>
+        <v>4410</v>
       </c>
     </row>
     <row r="2525" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34364,7 +34415,7 @@
         <v>2402</v>
       </c>
       <c r="B2525" s="1" t="s">
-        <v>4407</v>
+        <v>2402</v>
       </c>
     </row>
     <row r="2526" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34372,15 +34423,15 @@
         <v>2403</v>
       </c>
       <c r="B2526" s="1" t="s">
-        <v>4407</v>
-      </c>
-    </row>
-    <row r="2527" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>4411</v>
+      </c>
+    </row>
+    <row r="2527" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2527" s="1" t="s">
         <v>2404</v>
       </c>
       <c r="B2527" s="1" t="s">
-        <v>4413</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="2528" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34388,7 +34439,7 @@
         <v>2405</v>
       </c>
       <c r="B2528" s="1" t="s">
-        <v>2405</v>
+        <v>4409</v>
       </c>
     </row>
     <row r="2529" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34396,15 +34447,15 @@
         <v>2406</v>
       </c>
       <c r="B2529" s="1" t="s">
-        <v>4414</v>
-      </c>
-    </row>
-    <row r="2530" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>2406</v>
+      </c>
+    </row>
+    <row r="2530" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2530" s="1" t="s">
         <v>2407</v>
       </c>
       <c r="B2530" s="1" t="s">
-        <v>2407</v>
+        <v>4410</v>
       </c>
     </row>
     <row r="2531" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34412,7 +34463,7 @@
         <v>2408</v>
       </c>
       <c r="B2531" s="1" t="s">
-        <v>4412</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="2532" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34420,15 +34471,15 @@
         <v>2409</v>
       </c>
       <c r="B2532" s="1" t="s">
-        <v>2409</v>
-      </c>
-    </row>
-    <row r="2533" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>4411</v>
+      </c>
+    </row>
+    <row r="2533" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2533" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="B2533" s="1" t="s">
-        <v>4413</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="2534" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34436,7 +34487,7 @@
         <v>2411</v>
       </c>
       <c r="B2534" s="1" t="s">
-        <v>2411</v>
+        <v>4409</v>
       </c>
     </row>
     <row r="2535" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34444,15 +34495,15 @@
         <v>2412</v>
       </c>
       <c r="B2535" s="1" t="s">
-        <v>4414</v>
-      </c>
-    </row>
-    <row r="2536" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>2412</v>
+      </c>
+    </row>
+    <row r="2536" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2536" s="1" t="s">
         <v>2413</v>
       </c>
       <c r="B2536" s="1" t="s">
-        <v>2413</v>
+        <v>4412</v>
       </c>
     </row>
     <row r="2537" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34460,7 +34511,7 @@
         <v>2414</v>
       </c>
       <c r="B2537" s="1" t="s">
-        <v>4412</v>
+        <v>2414</v>
       </c>
     </row>
     <row r="2538" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34471,76 +34522,76 @@
         <v>2415</v>
       </c>
     </row>
-    <row r="2539" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2539" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2539" s="1" t="s">
         <v>2416</v>
       </c>
       <c r="B2539" s="1" t="s">
-        <v>4415</v>
-      </c>
-    </row>
-    <row r="2540" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>2416</v>
+      </c>
+    </row>
+    <row r="2540" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2540" s="1" t="s">
         <v>2417</v>
       </c>
       <c r="B2540" s="1" t="s">
-        <v>2417</v>
-      </c>
-    </row>
-    <row r="2541" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4413</v>
+      </c>
+    </row>
+    <row r="2541" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2541" s="1" t="s">
         <v>2418</v>
       </c>
       <c r="B2541" s="1" t="s">
-        <v>2418</v>
-      </c>
-    </row>
-    <row r="2542" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4413</v>
+      </c>
+    </row>
+    <row r="2542" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2542" s="1" t="s">
         <v>2419</v>
       </c>
       <c r="B2542" s="1" t="s">
-        <v>2419</v>
-      </c>
-    </row>
-    <row r="2543" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>4412</v>
+      </c>
+    </row>
+    <row r="2543" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2543" s="1" t="s">
         <v>2420</v>
       </c>
       <c r="B2543" s="1" t="s">
-        <v>4416</v>
-      </c>
-    </row>
-    <row r="2544" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="2544" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2544" s="1" t="s">
         <v>2421</v>
       </c>
       <c r="B2544" s="1" t="s">
-        <v>4416</v>
-      </c>
-    </row>
-    <row r="2545" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>2421</v>
+      </c>
+    </row>
+    <row r="2545" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2545" s="1" t="s">
         <v>2422</v>
       </c>
       <c r="B2545" s="1" t="s">
-        <v>4415</v>
-      </c>
-    </row>
-    <row r="2546" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>2422</v>
+      </c>
+    </row>
+    <row r="2546" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2546" s="1" t="s">
         <v>2423</v>
       </c>
       <c r="B2546" s="1" t="s">
-        <v>2423</v>
-      </c>
-    </row>
-    <row r="2547" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4413</v>
+      </c>
+    </row>
+    <row r="2547" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2547" s="1" t="s">
         <v>2424</v>
       </c>
       <c r="B2547" s="1" t="s">
-        <v>2424</v>
+        <v>4412</v>
       </c>
     </row>
     <row r="2548" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34551,28 +34602,28 @@
         <v>2425</v>
       </c>
     </row>
-    <row r="2549" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2549" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2549" s="1" t="s">
         <v>2426</v>
       </c>
       <c r="B2549" s="1" t="s">
-        <v>4416</v>
-      </c>
-    </row>
-    <row r="2550" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>4414</v>
+      </c>
+    </row>
+    <row r="2550" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2550" s="1" t="s">
         <v>2427</v>
       </c>
       <c r="B2550" s="1" t="s">
-        <v>4415</v>
-      </c>
-    </row>
-    <row r="2551" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>2427</v>
+      </c>
+    </row>
+    <row r="2551" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2551" s="1" t="s">
         <v>2428</v>
       </c>
       <c r="B2551" s="1" t="s">
-        <v>2428</v>
+        <v>4415</v>
       </c>
     </row>
     <row r="2552" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34580,7 +34631,7 @@
         <v>2429</v>
       </c>
       <c r="B2552" s="1" t="s">
-        <v>4417</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="2553" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34588,15 +34639,15 @@
         <v>2430</v>
       </c>
       <c r="B2553" s="1" t="s">
-        <v>2430</v>
-      </c>
-    </row>
-    <row r="2554" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>4414</v>
+      </c>
+    </row>
+    <row r="2554" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2554" s="1" t="s">
         <v>2431</v>
       </c>
       <c r="B2554" s="1" t="s">
-        <v>4418</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="2555" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34604,7 +34655,7 @@
         <v>2432</v>
       </c>
       <c r="B2555" s="1" t="s">
-        <v>2432</v>
+        <v>4414</v>
       </c>
     </row>
     <row r="2556" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34612,7 +34663,7 @@
         <v>2433</v>
       </c>
       <c r="B2556" s="1" t="s">
-        <v>4417</v>
+        <v>2433</v>
       </c>
     </row>
     <row r="2557" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34628,15 +34679,15 @@
         <v>2435</v>
       </c>
       <c r="B2558" s="1" t="s">
-        <v>4417</v>
-      </c>
-    </row>
-    <row r="2559" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4414</v>
+      </c>
+    </row>
+    <row r="2559" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2559" s="1" t="s">
         <v>2436</v>
       </c>
       <c r="B2559" s="1" t="s">
-        <v>2436</v>
+        <v>4416</v>
       </c>
     </row>
     <row r="2560" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34644,7 +34695,7 @@
         <v>2437</v>
       </c>
       <c r="B2560" s="1" t="s">
-        <v>2437</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="2561" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34652,15 +34703,15 @@
         <v>2438</v>
       </c>
       <c r="B2561" s="1" t="s">
-        <v>4417</v>
-      </c>
-    </row>
-    <row r="2562" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="2562" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2562" s="1" t="s">
         <v>2439</v>
       </c>
       <c r="B2562" s="1" t="s">
-        <v>4419</v>
+        <v>2439</v>
       </c>
     </row>
     <row r="2563" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34668,7 +34719,7 @@
         <v>2440</v>
       </c>
       <c r="B2563" s="1" t="s">
-        <v>4420</v>
+        <v>2440</v>
       </c>
     </row>
     <row r="2564" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34676,15 +34727,15 @@
         <v>2441</v>
       </c>
       <c r="B2564" s="1" t="s">
-        <v>2441</v>
-      </c>
-    </row>
-    <row r="2565" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4418</v>
+      </c>
+    </row>
+    <row r="2565" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2565" s="1" t="s">
         <v>2442</v>
       </c>
       <c r="B2565" s="1" t="s">
-        <v>2442</v>
+        <v>4416</v>
       </c>
     </row>
     <row r="2566" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34692,7 +34743,7 @@
         <v>2443</v>
       </c>
       <c r="B2566" s="1" t="s">
-        <v>2443</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="2567" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34700,15 +34751,15 @@
         <v>2444</v>
       </c>
       <c r="B2567" s="1" t="s">
-        <v>4421</v>
-      </c>
-    </row>
-    <row r="2568" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>2444</v>
+      </c>
+    </row>
+    <row r="2568" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2568" s="1" t="s">
         <v>2445</v>
       </c>
       <c r="B2568" s="1" t="s">
-        <v>4419</v>
+        <v>2445</v>
       </c>
     </row>
     <row r="2569" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34716,7 +34767,7 @@
         <v>2446</v>
       </c>
       <c r="B2569" s="1" t="s">
-        <v>4420</v>
+        <v>2446</v>
       </c>
     </row>
     <row r="2570" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34724,15 +34775,15 @@
         <v>2447</v>
       </c>
       <c r="B2570" s="1" t="s">
-        <v>2447</v>
-      </c>
-    </row>
-    <row r="2571" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4418</v>
+      </c>
+    </row>
+    <row r="2571" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2571" s="1" t="s">
         <v>2448</v>
       </c>
       <c r="B2571" s="1" t="s">
-        <v>2448</v>
+        <v>4422</v>
       </c>
     </row>
     <row r="2572" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34743,7 +34794,7 @@
         <v>2449</v>
       </c>
     </row>
-    <row r="2573" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2573" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2573" s="1" t="s">
         <v>2450</v>
       </c>
@@ -34751,12 +34802,12 @@
         <v>4421</v>
       </c>
     </row>
-    <row r="2574" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2574" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2574" s="1" t="s">
         <v>2451</v>
       </c>
       <c r="B2574" s="1" t="s">
-        <v>4425</v>
+        <v>2451</v>
       </c>
     </row>
     <row r="2575" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34764,23 +34815,23 @@
         <v>2452</v>
       </c>
       <c r="B2575" s="1" t="s">
-        <v>2452</v>
-      </c>
-    </row>
-    <row r="2576" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>4423</v>
+      </c>
+    </row>
+    <row r="2576" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2576" s="1" t="s">
         <v>2453</v>
       </c>
       <c r="B2576" s="1" t="s">
-        <v>4424</v>
-      </c>
-    </row>
-    <row r="2577" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>2453</v>
+      </c>
+    </row>
+    <row r="2577" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2577" s="1" t="s">
         <v>2454</v>
       </c>
       <c r="B2577" s="1" t="s">
-        <v>2454</v>
+        <v>4422</v>
       </c>
     </row>
     <row r="2578" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34788,23 +34839,23 @@
         <v>2455</v>
       </c>
       <c r="B2578" s="1" t="s">
-        <v>4426</v>
-      </c>
-    </row>
-    <row r="2579" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>2455</v>
+      </c>
+    </row>
+    <row r="2579" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2579" s="1" t="s">
         <v>2456</v>
       </c>
       <c r="B2579" s="1" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2580" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>4421</v>
+      </c>
+    </row>
+    <row r="2580" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2580" s="1" t="s">
         <v>2457</v>
       </c>
       <c r="B2580" s="1" t="s">
-        <v>4425</v>
+        <v>2457</v>
       </c>
     </row>
     <row r="2581" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34812,23 +34863,23 @@
         <v>2458</v>
       </c>
       <c r="B2581" s="1" t="s">
-        <v>2458</v>
-      </c>
-    </row>
-    <row r="2582" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>4423</v>
+      </c>
+    </row>
+    <row r="2582" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2582" s="1" t="s">
         <v>2459</v>
       </c>
       <c r="B2582" s="1" t="s">
-        <v>4424</v>
-      </c>
-    </row>
-    <row r="2583" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>2459</v>
+      </c>
+    </row>
+    <row r="2583" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2583" s="1" t="s">
         <v>2460</v>
       </c>
       <c r="B2583" s="1" t="s">
-        <v>2460</v>
+        <v>4424</v>
       </c>
     </row>
     <row r="2584" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34836,71 +34887,71 @@
         <v>2461</v>
       </c>
       <c r="B2584" s="1" t="s">
-        <v>4426</v>
-      </c>
-    </row>
-    <row r="2585" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>2461</v>
+      </c>
+    </row>
+    <row r="2585" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2585" s="1" t="s">
         <v>2462</v>
       </c>
       <c r="B2585" s="1" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2586" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>4425</v>
+      </c>
+    </row>
+    <row r="2586" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2586" s="1" t="s">
         <v>2463</v>
       </c>
       <c r="B2586" s="1" t="s">
-        <v>4427</v>
-      </c>
-    </row>
-    <row r="2587" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>2463</v>
+      </c>
+    </row>
+    <row r="2587" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2587" s="1" t="s">
         <v>2464</v>
       </c>
       <c r="B2587" s="1" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2588" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>4426</v>
+      </c>
+    </row>
+    <row r="2588" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2588" s="1" t="s">
         <v>2465</v>
       </c>
       <c r="B2588" s="1" t="s">
-        <v>4428</v>
-      </c>
-    </row>
-    <row r="2589" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>2465</v>
+      </c>
+    </row>
+    <row r="2589" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2589" s="1" t="s">
         <v>2466</v>
       </c>
       <c r="B2589" s="1" t="s">
-        <v>2466</v>
-      </c>
-    </row>
-    <row r="2590" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>4424</v>
+      </c>
+    </row>
+    <row r="2590" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2590" s="1" t="s">
         <v>2467</v>
       </c>
       <c r="B2590" s="1" t="s">
-        <v>4429</v>
-      </c>
-    </row>
-    <row r="2591" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>2467</v>
+      </c>
+    </row>
+    <row r="2591" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2591" s="1" t="s">
         <v>2468</v>
       </c>
       <c r="B2591" s="1" t="s">
-        <v>2468</v>
-      </c>
-    </row>
-    <row r="2592" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>4425</v>
+      </c>
+    </row>
+    <row r="2592" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2592" s="1" t="s">
         <v>2469</v>
       </c>
       <c r="B2592" s="1" t="s">
-        <v>4427</v>
+        <v>2469</v>
       </c>
     </row>
     <row r="2593" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -34911,12 +34962,12 @@
         <v>2470</v>
       </c>
     </row>
-    <row r="2594" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2594" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2594" s="1" t="s">
         <v>2471</v>
       </c>
       <c r="B2594" s="1" t="s">
-        <v>4428</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="2595" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -36655,12 +36706,12 @@
         <v>2688</v>
       </c>
     </row>
-    <row r="2812" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2812" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2812" s="1" t="s">
         <v>2689</v>
       </c>
       <c r="B2812" s="1" t="s">
-        <v>2689</v>
+        <v>4408</v>
       </c>
     </row>
     <row r="2813" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -36679,12 +36730,12 @@
         <v>2691</v>
       </c>
     </row>
-    <row r="2815" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2815" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2815" s="1" t="s">
         <v>2692</v>
       </c>
       <c r="B2815" s="1" t="s">
-        <v>4411</v>
+        <v>2692</v>
       </c>
     </row>
     <row r="2816" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -36708,7 +36759,7 @@
         <v>2695</v>
       </c>
       <c r="B2818" s="1" t="s">
-        <v>2695</v>
+        <v>4407</v>
       </c>
     </row>
     <row r="2819" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -36732,7 +36783,7 @@
         <v>2698</v>
       </c>
       <c r="B2821" s="1" t="s">
-        <v>4410</v>
+        <v>2698</v>
       </c>
     </row>
     <row r="2822" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -39495,12 +39546,12 @@
         <v>3043</v>
       </c>
     </row>
-    <row r="3167" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3167" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3167" s="1" t="s">
         <v>3044</v>
       </c>
       <c r="B3167" s="1" t="s">
-        <v>3044</v>
+        <v>4382</v>
       </c>
     </row>
     <row r="3168" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -39519,12 +39570,12 @@
         <v>3046</v>
       </c>
     </row>
-    <row r="3170" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3170" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3170" s="1" t="s">
         <v>3047</v>
       </c>
       <c r="B3170" s="1" t="s">
-        <v>4385</v>
+        <v>3047</v>
       </c>
     </row>
     <row r="3171" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -43703,31 +43754,31 @@
         <v>3569</v>
       </c>
     </row>
-    <row r="3693" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3693" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3693" s="1" t="s">
-        <v>3570</v>
+        <v>3691</v>
       </c>
       <c r="B3693" s="1" t="s">
-        <v>3570</v>
+        <v>3691</v>
       </c>
     </row>
     <row r="3694" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3694" s="1" t="s">
-        <v>3571</v>
+        <v>3692</v>
       </c>
       <c r="B3694" s="1" t="s">
-        <v>3571</v>
-      </c>
-    </row>
-    <row r="3695" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>3692</v>
+      </c>
+    </row>
+    <row r="3695" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3695" s="1" t="s">
-        <v>3572</v>
+        <v>3693</v>
       </c>
       <c r="B3695" s="1" t="s">
-        <v>3572</v>
-      </c>
-    </row>
-    <row r="3696" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3693</v>
+      </c>
+    </row>
+    <row r="3696" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3696" s="1" t="s">
         <v>3694</v>
       </c>
@@ -43735,7 +43786,7 @@
         <v>3694</v>
       </c>
     </row>
-    <row r="3697" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3697" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3697" s="1" t="s">
         <v>3695</v>
       </c>
@@ -43743,7 +43794,7 @@
         <v>3695</v>
       </c>
     </row>
-    <row r="3698" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3698" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3698" s="1" t="s">
         <v>3696</v>
       </c>
@@ -43759,7 +43810,7 @@
         <v>3697</v>
       </c>
     </row>
-    <row r="3700" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3700" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3700" s="1" t="s">
         <v>3698</v>
       </c>
@@ -43775,7 +43826,7 @@
         <v>3699</v>
       </c>
     </row>
-    <row r="3702" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3702" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3702" s="1" t="s">
         <v>3700</v>
       </c>
@@ -44287,7 +44338,7 @@
         <v>3763</v>
       </c>
     </row>
-    <row r="3766" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3766" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3766" s="1" t="s">
         <v>3764</v>
       </c>
@@ -44311,7 +44362,7 @@
         <v>3766</v>
       </c>
     </row>
-    <row r="3769" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3769" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3769" s="1" t="s">
         <v>3767</v>
       </c>
@@ -44375,7 +44426,7 @@
         <v>3774</v>
       </c>
     </row>
-    <row r="3777" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3777" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3777" s="1" t="s">
         <v>3775</v>
       </c>
@@ -44399,7 +44450,7 @@
         <v>3777</v>
       </c>
     </row>
-    <row r="3780" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3780" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3780" s="1" t="s">
         <v>3778</v>
       </c>
@@ -44463,7 +44514,7 @@
         <v>3785</v>
       </c>
     </row>
-    <row r="3788" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3788" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3788" s="1" t="s">
         <v>3786</v>
       </c>
@@ -44487,7 +44538,7 @@
         <v>3788</v>
       </c>
     </row>
-    <row r="3791" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3791" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3791" s="1" t="s">
         <v>3789</v>
       </c>
@@ -44551,7 +44602,7 @@
         <v>3796</v>
       </c>
     </row>
-    <row r="3799" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3799" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3799" s="1" t="s">
         <v>3797</v>
       </c>
@@ -44575,7 +44626,7 @@
         <v>3799</v>
       </c>
     </row>
-    <row r="3802" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3802" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3802" s="1" t="s">
         <v>3800</v>
       </c>
@@ -44639,7 +44690,7 @@
         <v>3807</v>
       </c>
     </row>
-    <row r="3810" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3810" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3810" s="1" t="s">
         <v>3808</v>
       </c>
@@ -44663,7 +44714,7 @@
         <v>3810</v>
       </c>
     </row>
-    <row r="3813" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3813" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3813" s="1" t="s">
         <v>3811</v>
       </c>
@@ -44727,7 +44778,7 @@
         <v>3818</v>
       </c>
     </row>
-    <row r="3821" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3821" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3821" s="1" t="s">
         <v>3819</v>
       </c>
@@ -44751,7 +44802,7 @@
         <v>3821</v>
       </c>
     </row>
-    <row r="3824" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3824" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3824" s="1" t="s">
         <v>3822</v>
       </c>
@@ -44807,7 +44858,7 @@
         <v>3828</v>
       </c>
     </row>
-    <row r="3831" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3831" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3831" s="1" t="s">
         <v>3829</v>
       </c>
@@ -44831,7 +44882,7 @@
         <v>3831</v>
       </c>
     </row>
-    <row r="3834" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3834" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3834" s="1" t="s">
         <v>3832</v>
       </c>
@@ -44895,7 +44946,7 @@
         <v>3839</v>
       </c>
     </row>
-    <row r="3842" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3842" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3842" s="1" t="s">
         <v>3840</v>
       </c>
@@ -44919,7 +44970,7 @@
         <v>3842</v>
       </c>
     </row>
-    <row r="3845" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3845" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3845" s="1" t="s">
         <v>3843</v>
       </c>
@@ -44991,7 +45042,7 @@
         <v>3851</v>
       </c>
     </row>
-    <row r="3854" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3854" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3854" s="1" t="s">
         <v>3852</v>
       </c>
@@ -45015,7 +45066,7 @@
         <v>3854</v>
       </c>
     </row>
-    <row r="3857" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3857" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3857" s="1" t="s">
         <v>3855</v>
       </c>
@@ -45071,7 +45122,7 @@
         <v>3861</v>
       </c>
     </row>
-    <row r="3864" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3864" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3864" s="1" t="s">
         <v>3862</v>
       </c>
@@ -45095,7 +45146,7 @@
         <v>3864</v>
       </c>
     </row>
-    <row r="3867" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3867" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3867" s="1" t="s">
         <v>3865</v>
       </c>
@@ -45167,7 +45218,7 @@
         <v>3873</v>
       </c>
     </row>
-    <row r="3876" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3876" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3876" s="1" t="s">
         <v>3874</v>
       </c>
@@ -45191,7 +45242,7 @@
         <v>3876</v>
       </c>
     </row>
-    <row r="3879" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3879" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3879" s="1" t="s">
         <v>3877</v>
       </c>
@@ -45255,7 +45306,7 @@
         <v>3884</v>
       </c>
     </row>
-    <row r="3887" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3887" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3887" s="1" t="s">
         <v>3885</v>
       </c>
@@ -45279,7 +45330,7 @@
         <v>3887</v>
       </c>
     </row>
-    <row r="3890" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3890" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3890" s="1" t="s">
         <v>3888</v>
       </c>
@@ -45335,7 +45386,7 @@
         <v>3894</v>
       </c>
     </row>
-    <row r="3897" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3897" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3897" s="1" t="s">
         <v>3895</v>
       </c>
@@ -45359,7 +45410,7 @@
         <v>3897</v>
       </c>
     </row>
-    <row r="3900" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3900" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3900" s="1" t="s">
         <v>3898</v>
       </c>
@@ -45431,7 +45482,7 @@
         <v>3906</v>
       </c>
     </row>
-    <row r="3909" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3909" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3909" s="1" t="s">
         <v>3907</v>
       </c>
@@ -45455,7 +45506,7 @@
         <v>3909</v>
       </c>
     </row>
-    <row r="3912" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3912" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3912" s="1" t="s">
         <v>3910</v>
       </c>
@@ -45615,7 +45666,7 @@
         <v>3929</v>
       </c>
     </row>
-    <row r="3932" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3932" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3932" s="1" t="s">
         <v>3930</v>
       </c>
@@ -45639,7 +45690,7 @@
         <v>3932</v>
       </c>
     </row>
-    <row r="3935" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3935" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3935" s="1" t="s">
         <v>3933</v>
       </c>
@@ -45695,7 +45746,7 @@
         <v>3939</v>
       </c>
     </row>
-    <row r="3942" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3942" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3942" s="1" t="s">
         <v>3940</v>
       </c>
@@ -45719,7 +45770,7 @@
         <v>3942</v>
       </c>
     </row>
-    <row r="3945" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3945" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3945" s="1" t="s">
         <v>3943</v>
       </c>
@@ -45791,7 +45842,7 @@
         <v>3951</v>
       </c>
     </row>
-    <row r="3954" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3954" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3954" s="1" t="s">
         <v>3952</v>
       </c>
@@ -45815,7 +45866,7 @@
         <v>3954</v>
       </c>
     </row>
-    <row r="3957" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3957" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3957" s="1" t="s">
         <v>3955</v>
       </c>
@@ -45879,7 +45930,7 @@
         <v>3962</v>
       </c>
     </row>
-    <row r="3965" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3965" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3965" s="1" t="s">
         <v>3963</v>
       </c>
@@ -45903,7 +45954,7 @@
         <v>3965</v>
       </c>
     </row>
-    <row r="3968" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3968" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3968" s="1" t="s">
         <v>3966</v>
       </c>
@@ -45967,7 +46018,7 @@
         <v>3973</v>
       </c>
     </row>
-    <row r="3976" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3976" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3976" s="1" t="s">
         <v>3974</v>
       </c>
@@ -45991,7 +46042,7 @@
         <v>3976</v>
       </c>
     </row>
-    <row r="3979" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3979" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3979" s="1" t="s">
         <v>3977</v>
       </c>
@@ -46063,7 +46114,7 @@
         <v>3985</v>
       </c>
     </row>
-    <row r="3988" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3988" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3988" s="1" t="s">
         <v>3986</v>
       </c>
@@ -46087,7 +46138,7 @@
         <v>3988</v>
       </c>
     </row>
-    <row r="3991" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3991" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3991" s="1" t="s">
         <v>3989</v>
       </c>
@@ -46151,7 +46202,7 @@
         <v>3996</v>
       </c>
     </row>
-    <row r="3999" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3999" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3999" s="1" t="s">
         <v>3997</v>
       </c>
@@ -46175,7 +46226,7 @@
         <v>3999</v>
       </c>
     </row>
-    <row r="4002" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4002" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4002" s="1" t="s">
         <v>4000</v>
       </c>
@@ -46239,7 +46290,7 @@
         <v>4007</v>
       </c>
     </row>
-    <row r="4010" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4010" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4010" s="1" t="s">
         <v>4008</v>
       </c>
@@ -46263,7 +46314,7 @@
         <v>4010</v>
       </c>
     </row>
-    <row r="4013" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4013" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4013" s="1" t="s">
         <v>4011</v>
       </c>
@@ -46327,7 +46378,7 @@
         <v>4018</v>
       </c>
     </row>
-    <row r="4021" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4021" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4021" s="1" t="s">
         <v>4019</v>
       </c>
@@ -46351,7 +46402,7 @@
         <v>4021</v>
       </c>
     </row>
-    <row r="4024" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4024" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4024" s="1" t="s">
         <v>4022</v>
       </c>
@@ -46415,7 +46466,7 @@
         <v>4029</v>
       </c>
     </row>
-    <row r="4032" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4032" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4032" s="1" t="s">
         <v>4030</v>
       </c>
@@ -46439,7 +46490,7 @@
         <v>4032</v>
       </c>
     </row>
-    <row r="4035" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4035" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4035" s="1" t="s">
         <v>4033</v>
       </c>
@@ -46503,7 +46554,7 @@
         <v>4040</v>
       </c>
     </row>
-    <row r="4043" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4043" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4043" s="1" t="s">
         <v>4041</v>
       </c>
@@ -46527,7 +46578,7 @@
         <v>4043</v>
       </c>
     </row>
-    <row r="4046" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4046" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4046" s="1" t="s">
         <v>4044</v>
       </c>
@@ -46599,7 +46650,7 @@
         <v>4052</v>
       </c>
     </row>
-    <row r="4055" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4055" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4055" s="1" t="s">
         <v>4053</v>
       </c>
@@ -46623,7 +46674,7 @@
         <v>4055</v>
       </c>
     </row>
-    <row r="4058" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4058" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4058" s="1" t="s">
         <v>4056</v>
       </c>
@@ -46687,7 +46738,7 @@
         <v>4063</v>
       </c>
     </row>
-    <row r="4066" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4066" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4066" s="1" t="s">
         <v>4064</v>
       </c>
@@ -46711,7 +46762,7 @@
         <v>4066</v>
       </c>
     </row>
-    <row r="4069" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4069" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4069" s="1" t="s">
         <v>4067</v>
       </c>
@@ -46783,7 +46834,7 @@
         <v>4075</v>
       </c>
     </row>
-    <row r="4078" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4078" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4078" s="1" t="s">
         <v>4076</v>
       </c>
@@ -46807,7 +46858,7 @@
         <v>4078</v>
       </c>
     </row>
-    <row r="4081" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4081" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4081" s="1" t="s">
         <v>4079</v>
       </c>
@@ -46871,7 +46922,7 @@
         <v>4086</v>
       </c>
     </row>
-    <row r="4089" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4089" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4089" s="1" t="s">
         <v>4087</v>
       </c>
@@ -46895,7 +46946,7 @@
         <v>4089</v>
       </c>
     </row>
-    <row r="4092" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4092" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4092" s="1" t="s">
         <v>4090</v>
       </c>
@@ -46967,7 +47018,7 @@
         <v>4098</v>
       </c>
     </row>
-    <row r="4101" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4101" s="1" t="s">
         <v>4099</v>
       </c>
@@ -46991,7 +47042,7 @@
         <v>4101</v>
       </c>
     </row>
-    <row r="4104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4104" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4104" s="1" t="s">
         <v>4102</v>
       </c>
@@ -47047,7 +47098,7 @@
         <v>4108</v>
       </c>
     </row>
-    <row r="4111" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4111" s="1" t="s">
         <v>4109</v>
       </c>
@@ -47071,7 +47122,7 @@
         <v>4111</v>
       </c>
     </row>
-    <row r="4114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4114" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4114" s="1" t="s">
         <v>4112</v>
       </c>
@@ -47311,7 +47362,7 @@
         <v>4141</v>
       </c>
     </row>
-    <row r="4144" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4144" s="1" t="s">
         <v>4142</v>
       </c>
@@ -47335,7 +47386,7 @@
         <v>4144</v>
       </c>
     </row>
-    <row r="4147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4147" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4147" s="1" t="s">
         <v>4145</v>
       </c>
@@ -47407,7 +47458,7 @@
         <v>4153</v>
       </c>
     </row>
-    <row r="4156" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4156" s="1" t="s">
         <v>4154</v>
       </c>
@@ -47431,7 +47482,7 @@
         <v>4156</v>
       </c>
     </row>
-    <row r="4159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4159" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4159" s="1" t="s">
         <v>4157</v>
       </c>
@@ -47495,7 +47546,7 @@
         <v>4164</v>
       </c>
     </row>
-    <row r="4167" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4167" s="1" t="s">
         <v>4165</v>
       </c>
@@ -47519,7 +47570,7 @@
         <v>4167</v>
       </c>
     </row>
-    <row r="4170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4170" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4170" s="1" t="s">
         <v>4168</v>
       </c>
@@ -47535,7 +47586,7 @@
         <v>4169</v>
       </c>
     </row>
-    <row r="4172" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4172" s="1" t="s">
         <v>4170</v>
       </c>
@@ -47543,7 +47594,7 @@
         <v>4170</v>
       </c>
     </row>
-    <row r="4173" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4173" s="1" t="s">
         <v>4171</v>
       </c>
@@ -47551,7 +47602,7 @@
         <v>4171</v>
       </c>
     </row>
-    <row r="4174" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4174" s="1" t="s">
         <v>4172</v>
       </c>
@@ -47572,7 +47623,7 @@
         <v>4174</v>
       </c>
       <c r="B4176" s="1" t="s">
-        <v>4174</v>
+        <v>4427</v>
       </c>
     </row>
     <row r="4177" spans="1:2" x14ac:dyDescent="0.25">
@@ -47596,7 +47647,7 @@
         <v>4177</v>
       </c>
       <c r="B4179" s="1" t="s">
-        <v>4430</v>
+        <v>4435</v>
       </c>
     </row>
     <row r="4180" spans="1:2" x14ac:dyDescent="0.25">
@@ -47612,7 +47663,7 @@
         <v>4179</v>
       </c>
       <c r="B4181" s="1" t="s">
-        <v>4179</v>
+        <v>4437</v>
       </c>
     </row>
     <row r="4182" spans="1:2" x14ac:dyDescent="0.25">
@@ -47620,7 +47671,7 @@
         <v>4180</v>
       </c>
       <c r="B4182" s="1" t="s">
-        <v>4438</v>
+        <v>4180</v>
       </c>
     </row>
     <row r="4183" spans="1:2" x14ac:dyDescent="0.25">
@@ -47636,7 +47687,7 @@
         <v>4182</v>
       </c>
       <c r="B4184" s="1" t="s">
-        <v>4440</v>
+        <v>4182</v>
       </c>
     </row>
     <row r="4185" spans="1:2" x14ac:dyDescent="0.25">
@@ -47679,7 +47730,7 @@
         <v>4187</v>
       </c>
     </row>
-    <row r="4190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4190" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4190" s="1" t="s">
         <v>4188</v>
       </c>
@@ -47687,7 +47738,7 @@
         <v>4188</v>
       </c>
     </row>
-    <row r="4191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4191" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4191" s="1" t="s">
         <v>4189</v>
       </c>
@@ -47727,7 +47778,7 @@
         <v>4193</v>
       </c>
     </row>
-    <row r="4196" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4196" s="1" t="s">
         <v>4194</v>
       </c>
@@ -47735,7 +47786,7 @@
         <v>4194</v>
       </c>
     </row>
-    <row r="4197" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4197" s="1" t="s">
         <v>4195</v>
       </c>
@@ -47991,12 +48042,12 @@
         <v>4226</v>
       </c>
     </row>
-    <row r="4229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4229" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4229" s="1" t="s">
         <v>4227</v>
       </c>
       <c r="B4229" s="1" t="s">
-        <v>4227</v>
+        <v>4428</v>
       </c>
     </row>
     <row r="4230" spans="1:2" x14ac:dyDescent="0.25">
@@ -48015,12 +48066,12 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="4232" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4232" s="1" t="s">
         <v>4230</v>
       </c>
       <c r="B4232" s="1" t="s">
-        <v>4431</v>
+        <v>4230</v>
       </c>
     </row>
     <row r="4233" spans="1:2" x14ac:dyDescent="0.25">
@@ -48039,7 +48090,7 @@
         <v>4232</v>
       </c>
     </row>
-    <row r="4235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4235" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4235" s="1" t="s">
         <v>4233</v>
       </c>
@@ -48068,7 +48119,7 @@
         <v>4236</v>
       </c>
       <c r="B4238" s="1" t="s">
-        <v>4236</v>
+        <v>4436</v>
       </c>
     </row>
     <row r="4239" spans="1:2" x14ac:dyDescent="0.25">
@@ -48087,12 +48138,12 @@
         <v>4238</v>
       </c>
     </row>
-    <row r="4241" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4241" s="1" t="s">
         <v>4239</v>
       </c>
       <c r="B4241" s="1" t="s">
-        <v>4439</v>
+        <v>4239</v>
       </c>
     </row>
     <row r="4242" spans="1:2" x14ac:dyDescent="0.25">
@@ -48167,7 +48218,7 @@
         <v>4248</v>
       </c>
     </row>
-    <row r="4251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4251" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4251" s="1" t="s">
         <v>4249</v>
       </c>
@@ -48175,7 +48226,7 @@
         <v>4249</v>
       </c>
     </row>
-    <row r="4252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4252" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4252" s="1" t="s">
         <v>4250</v>
       </c>
@@ -48183,7 +48234,7 @@
         <v>4250</v>
       </c>
     </row>
-    <row r="4253" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4253" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4253" s="1" t="s">
         <v>4251</v>
       </c>
@@ -49007,232 +49058,208 @@
         <v>4353</v>
       </c>
     </row>
-    <row r="4356" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4356" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4356" s="1" t="s">
-        <v>4354</v>
+        <v>4358</v>
       </c>
       <c r="B4356" s="1" t="s">
-        <v>4354</v>
-      </c>
-    </row>
-    <row r="4357" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4357</v>
+      </c>
+    </row>
+    <row r="4357" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4357" s="1" t="s">
-        <v>4355</v>
+        <v>4360</v>
       </c>
       <c r="B4357" s="1" t="s">
-        <v>4355</v>
-      </c>
-    </row>
-    <row r="4358" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4361</v>
+      </c>
+    </row>
+    <row r="4358" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4358" s="1" t="s">
-        <v>4356</v>
+        <v>4362</v>
       </c>
       <c r="B4358" s="1" t="s">
-        <v>4356</v>
+        <v>4361</v>
       </c>
     </row>
     <row r="4359" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4359" s="1" t="s">
-        <v>4361</v>
+        <v>4363</v>
       </c>
       <c r="B4359" s="1" t="s">
-        <v>4360</v>
+        <v>4364</v>
       </c>
     </row>
     <row r="4360" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4360" s="1" t="s">
-        <v>4363</v>
+        <v>4365</v>
       </c>
       <c r="B4360" s="1" t="s">
-        <v>4364</v>
+        <v>4366</v>
       </c>
     </row>
     <row r="4361" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4361" s="1" t="s">
-        <v>4365</v>
+        <v>4368</v>
       </c>
       <c r="B4361" s="1" t="s">
-        <v>4364</v>
+        <v>4369</v>
       </c>
     </row>
     <row r="4362" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4362" s="1" t="s">
-        <v>4366</v>
+        <v>4370</v>
       </c>
       <c r="B4362" s="1" t="s">
-        <v>4367</v>
-      </c>
-    </row>
-    <row r="4363" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="4363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4363" s="1" t="s">
-        <v>4368</v>
+        <v>4372</v>
       </c>
       <c r="B4363" s="1" t="s">
-        <v>4369</v>
-      </c>
-    </row>
-    <row r="4364" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4373</v>
+      </c>
+    </row>
+    <row r="4364" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A4364" s="1" t="s">
-        <v>4371</v>
+        <v>4374</v>
       </c>
       <c r="B4364" s="1" t="s">
-        <v>4372</v>
-      </c>
-    </row>
-    <row r="4365" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4375</v>
+      </c>
+    </row>
+    <row r="4365" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A4365" s="1" t="s">
-        <v>4373</v>
+        <v>4376</v>
       </c>
       <c r="B4365" s="1" t="s">
-        <v>4374</v>
-      </c>
-    </row>
-    <row r="4366" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4377</v>
+      </c>
+    </row>
+    <row r="4366" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4366" s="1" t="s">
-        <v>4375</v>
+        <v>4383</v>
       </c>
       <c r="B4366" s="1" t="s">
-        <v>4376</v>
-      </c>
-    </row>
-    <row r="4367" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>4382</v>
+      </c>
+    </row>
+    <row r="4367" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A4367" s="1" t="s">
-        <v>4377</v>
+        <v>4385</v>
       </c>
       <c r="B4367" s="1" t="s">
-        <v>4378</v>
-      </c>
-    </row>
-    <row r="4368" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>4386</v>
+      </c>
+    </row>
+    <row r="4368" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4368" s="1" t="s">
-        <v>4379</v>
+        <v>4388</v>
       </c>
       <c r="B4368" s="1" t="s">
-        <v>4380</v>
+        <v>4389</v>
       </c>
     </row>
     <row r="4369" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4369" s="1" t="s">
-        <v>4386</v>
+        <v>4390</v>
       </c>
       <c r="B4369" s="1" t="s">
-        <v>4385</v>
-      </c>
-    </row>
-    <row r="4370" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>4389</v>
+      </c>
+    </row>
+    <row r="4370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4370" s="1" t="s">
-        <v>4388</v>
+        <v>4391</v>
       </c>
       <c r="B4370" s="1" t="s">
-        <v>4389</v>
+        <v>4392</v>
       </c>
     </row>
     <row r="4371" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4371" s="1" t="s">
-        <v>4391</v>
+        <v>4393</v>
       </c>
       <c r="B4371" s="1" t="s">
-        <v>4392</v>
+        <v>4394</v>
       </c>
     </row>
     <row r="4372" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4372" s="1" t="s">
-        <v>4393</v>
+        <v>4395</v>
       </c>
       <c r="B4372" s="1" t="s">
-        <v>4392</v>
-      </c>
-    </row>
-    <row r="4373" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4396</v>
+      </c>
+    </row>
+    <row r="4373" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4373" s="1" t="s">
-        <v>4394</v>
+        <v>4406</v>
       </c>
       <c r="B4373" s="1" t="s">
-        <v>4395</v>
+        <v>4382</v>
       </c>
     </row>
     <row r="4374" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4374" s="1" t="s">
-        <v>4396</v>
+        <v>4419</v>
       </c>
       <c r="B4374" s="1" t="s">
-        <v>4397</v>
+        <v>4420</v>
       </c>
     </row>
     <row r="4375" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4375" s="1" t="s">
-        <v>4398</v>
+        <v>4429</v>
       </c>
       <c r="B4375" s="1" t="s">
-        <v>4399</v>
+        <v>4431</v>
       </c>
     </row>
     <row r="4376" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4376" s="1" t="s">
-        <v>4409</v>
+        <v>4430</v>
       </c>
       <c r="B4376" s="1" t="s">
-        <v>4385</v>
-      </c>
-    </row>
-    <row r="4377" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4428</v>
+      </c>
+    </row>
+    <row r="4377" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4377" s="1" t="s">
-        <v>4422</v>
+        <v>4432</v>
       </c>
       <c r="B4377" s="1" t="s">
-        <v>4423</v>
-      </c>
-    </row>
-    <row r="4378" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4432</v>
+      </c>
+    </row>
+    <row r="4378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4378" s="1" t="s">
-        <v>4432</v>
+        <v>4433</v>
       </c>
       <c r="B4378" s="1" t="s">
         <v>4434</v>
       </c>
     </row>
-    <row r="4379" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4379" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4379" s="1" t="s">
-        <v>4433</v>
+        <v>4438</v>
       </c>
       <c r="B4379" s="1" t="s">
-        <v>4431</v>
-      </c>
-    </row>
-    <row r="4380" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4438</v>
+      </c>
+    </row>
+    <row r="4380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4380" s="1" t="s">
-        <v>4435</v>
+        <v>4439</v>
       </c>
       <c r="B4380" s="1" t="s">
-        <v>4435</v>
-      </c>
-    </row>
-    <row r="4381" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4381" s="1" t="s">
-        <v>4436</v>
-      </c>
-      <c r="B4381" s="1" t="s">
-        <v>4437</v>
-      </c>
-    </row>
-    <row r="4382" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4382" s="1" t="s">
-        <v>4441</v>
-      </c>
-      <c r="B4382" s="1" t="s">
-        <v>4441</v>
-      </c>
-    </row>
-    <row r="4383" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4383" s="1" t="s">
-        <v>4442</v>
-      </c>
-      <c r="B4383" s="1" t="s">
-        <v>4443</v>
+        <v>4440</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B4383" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
+  <autoFilter ref="A1:B4380" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
     <filterColumn colId="0">
       <customFilters>
         <customFilter val="*tại Thiên Di"/>
@@ -49263,10 +49290,10 @@
     <cfRule type="duplicateValues" dxfId="25" priority="8"/>
     <cfRule type="duplicateValues" dxfId="24" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3782:A3843">
+  <conditionalFormatting sqref="A3779:A3840">
     <cfRule type="duplicateValues" dxfId="23" priority="36"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6685:A1048576 A1769:A1773 A209:A1600 A1:A23 A25:A84 A143 A3404:A3781 A3844:A4141 A1603:A1631">
+  <conditionalFormatting sqref="A6682:A1048576 A1769:A1773 A209:A1600 A1:A23 A25:A84 A143 A3401:A3778 A3841:A4138 A1603:A1631">
     <cfRule type="duplicateValues" dxfId="22" priority="114"/>
     <cfRule type="duplicateValues" dxfId="21" priority="116"/>
   </conditionalFormatting>
@@ -49308,18 +49335,18 @@
   <conditionalFormatting sqref="B1647">
     <cfRule type="duplicateValues" dxfId="5" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3782:B3843">
+  <conditionalFormatting sqref="B3779:B3840">
     <cfRule type="duplicateValues" dxfId="4" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6685:B1048576 B1769:B1773 B1:B23 B25:B84 B143 B3404:B3781 B3844:B4141 B1603:B1631 B209:B1600">
+  <conditionalFormatting sqref="B6682:B1048576 B1769:B1773 B1:B23 B25:B84 B143 B3401:B3778 B3841:B4138 B1603:B1631 B209:B1600">
     <cfRule type="duplicateValues" dxfId="3" priority="23"/>
     <cfRule type="duplicateValues" dxfId="2" priority="24"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1774:A3301">
-    <cfRule type="duplicateValues" dxfId="1" priority="174"/>
+  <conditionalFormatting sqref="A1774:A3298">
+    <cfRule type="duplicateValues" dxfId="1" priority="272"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1774:B3301">
-    <cfRule type="duplicateValues" dxfId="0" priority="176"/>
+  <conditionalFormatting sqref="B1774:B3298">
+    <cfRule type="duplicateValues" dxfId="0" priority="274"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>